<commit_message>
V49 pix_mod & color_mod => pix_mod
</commit_message>
<xml_diff>
--- a/sac_v2_io.xlsx
+++ b/sac_v2_io.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\KXKMSACIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A50608-2B69-49D0-B6DB-D3A5EF8E0289}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC53EE4-27E8-43E7-AC83-1792E3665DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sac_v2" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="v2_006_h_s" sheetId="7" r:id="rId4"/>
     <sheet name="kxkm_esp32_BAR_h_s_006" sheetId="8" r:id="rId5"/>
     <sheet name="kxkm_esp32_16_osc_artnet_remote" sheetId="9" r:id="rId6"/>
-    <sheet name="SACIO" sheetId="10" r:id="rId7"/>
+    <sheet name="SACIO &lt; v 48" sheetId="10" r:id="rId7"/>
+    <sheet name="SACIO V49" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="121">
   <si>
     <t>ch</t>
   </si>
@@ -390,6 +391,12 @@
   <si>
     <t>force auto_lock</t>
   </si>
+  <si>
+    <t>1 color</t>
+  </si>
+  <si>
+    <t>2 colors</t>
+  </si>
 </sst>
 </file>
 
@@ -1386,7 +1393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="238">
+  <cellXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2098,6 +2105,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13377,11 +13417,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383CC9FB-8C86-44E3-87C1-8A5C3498F613}">
-  <dimension ref="A1:BD37"/>
+  <dimension ref="A1:BC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y5" sqref="Y5"/>
+      <selection pane="topRight" activeCell="Y30" sqref="Y30:Y32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13396,14 +13436,14 @@
     <col min="20" max="20" width="11.42578125" style="1"/>
     <col min="23" max="24" width="6.7109375" customWidth="1"/>
     <col min="34" max="35" width="6.7109375" customWidth="1"/>
-    <col min="48" max="49" width="6.7109375" style="2" customWidth="1"/>
-    <col min="50" max="50" width="11.42578125" style="2"/>
-    <col min="51" max="52" width="6.7109375" style="2" customWidth="1"/>
-    <col min="53" max="53" width="16.7109375" style="232" customWidth="1"/>
-    <col min="54" max="56" width="11.42578125" style="2"/>
+    <col min="47" max="48" width="6.7109375" style="2" customWidth="1"/>
+    <col min="49" max="49" width="11.42578125" style="2"/>
+    <col min="50" max="51" width="6.7109375" style="2" customWidth="1"/>
+    <col min="52" max="52" width="16.7109375" style="232" customWidth="1"/>
+    <col min="53" max="55" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -13463,45 +13503,44 @@
       <c r="AK1" s="83">
         <v>10</v>
       </c>
-      <c r="AL1" s="78"/>
-      <c r="AM1" s="84"/>
-      <c r="AN1" s="103">
+      <c r="AL1" s="84"/>
+      <c r="AM1" s="103">
         <v>11</v>
       </c>
-      <c r="AO1" s="104"/>
-      <c r="AP1" s="103">
+      <c r="AN1" s="104"/>
+      <c r="AO1" s="103">
         <v>12</v>
       </c>
-      <c r="AQ1" s="104"/>
-      <c r="AR1" s="103">
+      <c r="AP1" s="104"/>
+      <c r="AQ1" s="103">
         <v>13</v>
       </c>
-      <c r="AS1" s="104"/>
-      <c r="AT1" s="103">
+      <c r="AR1" s="104"/>
+      <c r="AS1" s="103">
         <v>14</v>
       </c>
-      <c r="AU1" s="104"/>
-      <c r="AV1" s="83">
+      <c r="AT1" s="104"/>
+      <c r="AU1" s="83">
         <v>15</v>
       </c>
-      <c r="AW1" s="78"/>
-      <c r="AX1" s="84"/>
-      <c r="AY1" s="83">
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="84"/>
+      <c r="AX1" s="83">
         <v>16</v>
       </c>
-      <c r="AZ1" s="78"/>
-      <c r="BA1" s="84"/>
+      <c r="AY1" s="78"/>
+      <c r="AZ1" s="84"/>
+      <c r="BA1" s="3">
+        <v>17</v>
+      </c>
       <c r="BB1" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BC1" s="3">
-        <v>18</v>
-      </c>
-      <c r="BD1" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -13571,45 +13610,44 @@
       <c r="AK2" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="87"/>
-      <c r="AM2" s="90"/>
-      <c r="AN2" s="99" t="s">
+      <c r="AL2" s="90"/>
+      <c r="AM2" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="AO2" s="100"/>
-      <c r="AP2" s="99" t="s">
+      <c r="AN2" s="100"/>
+      <c r="AO2" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="AQ2" s="100"/>
-      <c r="AR2" s="99" t="s">
+      <c r="AP2" s="100"/>
+      <c r="AQ2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="AS2" s="100"/>
-      <c r="AT2" s="99" t="s">
+      <c r="AR2" s="100"/>
+      <c r="AS2" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="AU2" s="100"/>
-      <c r="AV2" s="89" t="s">
+      <c r="AT2" s="100"/>
+      <c r="AU2" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="AW2" s="87"/>
-      <c r="AX2" s="90"/>
-      <c r="AY2" s="89" t="s">
+      <c r="AV2" s="87"/>
+      <c r="AW2" s="90"/>
+      <c r="AX2" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="AZ2" s="87"/>
-      <c r="BA2" s="90"/>
+      <c r="AY2" s="87"/>
+      <c r="AZ2" s="90"/>
+      <c r="BA2" s="51" t="s">
+        <v>81</v>
+      </c>
       <c r="BB2" s="51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="BC2" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="BD2" s="51" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" s="208"/>
       <c r="B3" s="106" t="s">
         <v>15</v>
@@ -13673,7 +13711,7 @@
         <v>10</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="Z3" s="74">
         <v>0</v>
@@ -13707,63 +13745,62 @@
       <c r="AK3" s="192" t="s">
         <v>94</v>
       </c>
-      <c r="AL3" s="193"/>
-      <c r="AM3" s="114" t="s">
+      <c r="AL3" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="AN3" s="215" t="s">
+      <c r="AM3" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="AO3" s="107" t="s">
+      <c r="AN3" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="AP3" s="213" t="s">
+      <c r="AO3" s="213" t="s">
         <v>15</v>
       </c>
-      <c r="AQ3" s="91" t="s">
+      <c r="AP3" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="AR3" s="213" t="s">
+      <c r="AQ3" s="213" t="s">
         <v>15</v>
       </c>
-      <c r="AS3" s="91" t="s">
+      <c r="AR3" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="AT3" s="213" t="s">
+      <c r="AS3" s="213" t="s">
         <v>15</v>
       </c>
-      <c r="AU3" s="91" t="s">
+      <c r="AT3" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="AV3" s="8">
+      <c r="AU3" s="8">
         <v>0</v>
       </c>
-      <c r="AW3" s="9">
+      <c r="AV3" s="9">
         <v>10</v>
       </c>
-      <c r="AX3" s="10" t="s">
+      <c r="AW3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="AY3" s="8">
+      <c r="AX3" s="8">
         <v>0</v>
       </c>
-      <c r="AZ3" s="9">
+      <c r="AY3" s="9">
         <v>10</v>
       </c>
-      <c r="BA3" s="233" t="s">
+      <c r="AZ3" s="233" t="s">
         <v>53</v>
       </c>
+      <c r="BA3" s="96" t="s">
+        <v>93</v>
+      </c>
       <c r="BB3" s="96" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="BC3" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="BD3" s="96" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="209"/>
       <c r="B4" s="108"/>
       <c r="C4" s="221">
@@ -13817,7 +13854,7 @@
         <v>20</v>
       </c>
       <c r="Y4" s="17" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="Z4" s="151"/>
       <c r="AA4" s="187"/>
@@ -13837,39 +13874,38 @@
         <v>40</v>
       </c>
       <c r="AK4" s="194"/>
-      <c r="AL4" s="195"/>
-      <c r="AM4" s="81"/>
-      <c r="AN4" s="216"/>
-      <c r="AO4" s="109"/>
-      <c r="AP4" s="214"/>
-      <c r="AQ4" s="92"/>
-      <c r="AR4" s="214"/>
-      <c r="AS4" s="92"/>
-      <c r="AT4" s="214"/>
-      <c r="AU4" s="92"/>
-      <c r="AV4" s="48">
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="216"/>
+      <c r="AN4" s="109"/>
+      <c r="AO4" s="214"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="214"/>
+      <c r="AR4" s="92"/>
+      <c r="AS4" s="214"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="48">
         <v>11</v>
       </c>
-      <c r="AW4" s="49">
+      <c r="AV4" s="49">
         <v>20</v>
       </c>
-      <c r="AX4" s="50" t="s">
+      <c r="AW4" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="AY4" s="13">
+      <c r="AX4" s="13">
         <v>11</v>
       </c>
-      <c r="AZ4" s="14">
+      <c r="AY4" s="14">
         <v>20</v>
       </c>
-      <c r="BA4" s="234" t="s">
+      <c r="AZ4" s="234" t="s">
         <v>74</v>
       </c>
+      <c r="BA4" s="97"/>
       <c r="BB4" s="97"/>
       <c r="BC4" s="97"/>
-      <c r="BD4" s="97"/>
-    </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="209"/>
       <c r="B5" s="108"/>
       <c r="C5" s="221">
@@ -13943,39 +13979,38 @@
         <v>41</v>
       </c>
       <c r="AK5" s="194"/>
-      <c r="AL5" s="195"/>
-      <c r="AM5" s="81"/>
-      <c r="AN5" s="216"/>
-      <c r="AO5" s="109"/>
-      <c r="AP5" s="214"/>
-      <c r="AQ5" s="92"/>
-      <c r="AR5" s="214"/>
-      <c r="AS5" s="92"/>
-      <c r="AT5" s="214"/>
-      <c r="AU5" s="92"/>
-      <c r="AV5" s="55">
+      <c r="AL5" s="81"/>
+      <c r="AM5" s="216"/>
+      <c r="AN5" s="109"/>
+      <c r="AO5" s="214"/>
+      <c r="AP5" s="92"/>
+      <c r="AQ5" s="214"/>
+      <c r="AR5" s="92"/>
+      <c r="AS5" s="214"/>
+      <c r="AT5" s="92"/>
+      <c r="AU5" s="55">
         <v>21</v>
       </c>
-      <c r="AW5" s="56">
+      <c r="AV5" s="56">
         <v>30</v>
       </c>
-      <c r="AX5" s="57" t="s">
+      <c r="AW5" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="AY5" s="13">
+      <c r="AX5" s="13">
         <v>21</v>
       </c>
-      <c r="AZ5" s="14">
+      <c r="AY5" s="14">
         <v>30</v>
       </c>
-      <c r="BA5" s="234" t="s">
+      <c r="AZ5" s="234" t="s">
         <v>75</v>
       </c>
+      <c r="BA5" s="97"/>
       <c r="BB5" s="97"/>
       <c r="BC5" s="97"/>
-      <c r="BD5" s="97"/>
-    </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" s="209"/>
       <c r="B6" s="108"/>
       <c r="C6" s="221">
@@ -14049,37 +14084,36 @@
         <v>42</v>
       </c>
       <c r="AK6" s="194"/>
-      <c r="AL6" s="195"/>
-      <c r="AM6" s="81"/>
-      <c r="AN6" s="216"/>
-      <c r="AO6" s="109"/>
-      <c r="AP6" s="214"/>
-      <c r="AQ6" s="92"/>
-      <c r="AR6" s="214"/>
-      <c r="AS6" s="92"/>
-      <c r="AT6" s="214"/>
-      <c r="AU6" s="92"/>
-      <c r="AV6" s="13">
+      <c r="AL6" s="81"/>
+      <c r="AM6" s="216"/>
+      <c r="AN6" s="109"/>
+      <c r="AO6" s="214"/>
+      <c r="AP6" s="92"/>
+      <c r="AQ6" s="214"/>
+      <c r="AR6" s="92"/>
+      <c r="AS6" s="214"/>
+      <c r="AT6" s="92"/>
+      <c r="AU6" s="13">
         <v>31</v>
       </c>
-      <c r="AW6" s="14">
+      <c r="AV6" s="14">
         <v>40</v>
       </c>
-      <c r="AX6" s="15"/>
-      <c r="AY6" s="13">
+      <c r="AW6" s="15"/>
+      <c r="AX6" s="13">
         <v>31</v>
       </c>
-      <c r="AZ6" s="14">
+      <c r="AY6" s="14">
         <v>40</v>
       </c>
-      <c r="BA6" s="234" t="s">
+      <c r="AZ6" s="234" t="s">
         <v>76</v>
       </c>
+      <c r="BA6" s="97"/>
       <c r="BB6" s="97"/>
       <c r="BC6" s="97"/>
-      <c r="BD6" s="97"/>
-    </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" s="209"/>
       <c r="B7" s="108"/>
       <c r="C7" s="221">
@@ -14147,37 +14181,36 @@
       <c r="AI7" s="112"/>
       <c r="AJ7" s="129"/>
       <c r="AK7" s="194"/>
-      <c r="AL7" s="195"/>
-      <c r="AM7" s="81"/>
-      <c r="AN7" s="216"/>
-      <c r="AO7" s="109"/>
-      <c r="AP7" s="214"/>
-      <c r="AQ7" s="92"/>
-      <c r="AR7" s="214"/>
-      <c r="AS7" s="92"/>
-      <c r="AT7" s="214"/>
-      <c r="AU7" s="92"/>
-      <c r="AV7" s="13">
+      <c r="AL7" s="81"/>
+      <c r="AM7" s="216"/>
+      <c r="AN7" s="109"/>
+      <c r="AO7" s="214"/>
+      <c r="AP7" s="92"/>
+      <c r="AQ7" s="214"/>
+      <c r="AR7" s="92"/>
+      <c r="AS7" s="214"/>
+      <c r="AT7" s="92"/>
+      <c r="AU7" s="13">
         <v>41</v>
       </c>
-      <c r="AW7" s="14">
+      <c r="AV7" s="14">
         <v>50</v>
       </c>
-      <c r="AX7" s="15"/>
-      <c r="AY7" s="13">
+      <c r="AW7" s="15"/>
+      <c r="AX7" s="13">
         <v>41</v>
       </c>
-      <c r="AZ7" s="14">
+      <c r="AY7" s="14">
         <v>50</v>
       </c>
-      <c r="BA7" s="234" t="s">
+      <c r="AZ7" s="234" t="s">
         <v>79</v>
       </c>
+      <c r="BA7" s="97"/>
       <c r="BB7" s="97"/>
       <c r="BC7" s="97"/>
-      <c r="BD7" s="97"/>
-    </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="209"/>
       <c r="B8" s="108"/>
       <c r="C8" s="221">
@@ -14245,37 +14278,36 @@
       <c r="AI8" s="112"/>
       <c r="AJ8" s="129"/>
       <c r="AK8" s="194"/>
-      <c r="AL8" s="195"/>
-      <c r="AM8" s="81"/>
-      <c r="AN8" s="216"/>
-      <c r="AO8" s="109"/>
-      <c r="AP8" s="214"/>
-      <c r="AQ8" s="92"/>
-      <c r="AR8" s="214"/>
-      <c r="AS8" s="92"/>
-      <c r="AT8" s="214"/>
-      <c r="AU8" s="92"/>
-      <c r="AV8" s="13">
+      <c r="AL8" s="81"/>
+      <c r="AM8" s="216"/>
+      <c r="AN8" s="109"/>
+      <c r="AO8" s="214"/>
+      <c r="AP8" s="92"/>
+      <c r="AQ8" s="214"/>
+      <c r="AR8" s="92"/>
+      <c r="AS8" s="214"/>
+      <c r="AT8" s="92"/>
+      <c r="AU8" s="13">
         <v>51</v>
       </c>
-      <c r="AW8" s="14">
+      <c r="AV8" s="14">
         <v>60</v>
       </c>
-      <c r="AX8" s="15"/>
-      <c r="AY8" s="13">
+      <c r="AW8" s="15"/>
+      <c r="AX8" s="13">
         <v>51</v>
       </c>
-      <c r="AZ8" s="14">
+      <c r="AY8" s="14">
         <v>60</v>
       </c>
-      <c r="BA8" s="234" t="s">
+      <c r="AZ8" s="234" t="s">
         <v>78</v>
       </c>
+      <c r="BA8" s="97"/>
       <c r="BB8" s="97"/>
       <c r="BC8" s="97"/>
-      <c r="BD8" s="97"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A9" s="209"/>
       <c r="B9" s="108"/>
       <c r="C9" s="221">
@@ -14328,7 +14360,7 @@
       <c r="X9" s="14">
         <v>70</v>
       </c>
-      <c r="Y9" s="17"/>
+      <c r="Y9" s="244"/>
       <c r="Z9" s="149"/>
       <c r="AA9" s="187"/>
       <c r="AB9" s="163"/>
@@ -14341,37 +14373,36 @@
       <c r="AI9" s="112"/>
       <c r="AJ9" s="129"/>
       <c r="AK9" s="194"/>
-      <c r="AL9" s="195"/>
-      <c r="AM9" s="81"/>
-      <c r="AN9" s="216"/>
-      <c r="AO9" s="109"/>
-      <c r="AP9" s="214"/>
-      <c r="AQ9" s="92"/>
-      <c r="AR9" s="214"/>
-      <c r="AS9" s="92"/>
-      <c r="AT9" s="214"/>
-      <c r="AU9" s="92"/>
-      <c r="AV9" s="13">
+      <c r="AL9" s="81"/>
+      <c r="AM9" s="216"/>
+      <c r="AN9" s="109"/>
+      <c r="AO9" s="214"/>
+      <c r="AP9" s="92"/>
+      <c r="AQ9" s="214"/>
+      <c r="AR9" s="92"/>
+      <c r="AS9" s="214"/>
+      <c r="AT9" s="92"/>
+      <c r="AU9" s="13">
         <v>61</v>
       </c>
-      <c r="AW9" s="14">
+      <c r="AV9" s="14">
         <v>70</v>
       </c>
-      <c r="AX9" s="15"/>
-      <c r="AY9" s="13">
+      <c r="AW9" s="15"/>
+      <c r="AX9" s="13">
         <v>61</v>
       </c>
-      <c r="AZ9" s="14">
+      <c r="AY9" s="14">
         <v>70</v>
       </c>
-      <c r="BA9" s="234" t="s">
+      <c r="AZ9" s="234" t="s">
         <v>77</v>
       </c>
+      <c r="BA9" s="97"/>
       <c r="BB9" s="97"/>
       <c r="BC9" s="97"/>
-      <c r="BD9" s="97"/>
-    </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" s="209"/>
       <c r="B10" s="108"/>
       <c r="C10" s="221">
@@ -14424,7 +14455,7 @@
       <c r="X10" s="14">
         <v>80</v>
       </c>
-      <c r="Y10" s="17"/>
+      <c r="Y10" s="245"/>
       <c r="Z10" s="149"/>
       <c r="AA10" s="187"/>
       <c r="AB10" s="163"/>
@@ -14437,35 +14468,34 @@
       <c r="AI10" s="112"/>
       <c r="AJ10" s="129"/>
       <c r="AK10" s="194"/>
-      <c r="AL10" s="195"/>
-      <c r="AM10" s="81"/>
-      <c r="AN10" s="216"/>
-      <c r="AO10" s="109"/>
-      <c r="AP10" s="214"/>
-      <c r="AQ10" s="92"/>
-      <c r="AR10" s="214"/>
-      <c r="AS10" s="92"/>
-      <c r="AT10" s="214"/>
-      <c r="AU10" s="92"/>
-      <c r="AV10" s="13">
+      <c r="AL10" s="81"/>
+      <c r="AM10" s="216"/>
+      <c r="AN10" s="109"/>
+      <c r="AO10" s="214"/>
+      <c r="AP10" s="92"/>
+      <c r="AQ10" s="214"/>
+      <c r="AR10" s="92"/>
+      <c r="AS10" s="214"/>
+      <c r="AT10" s="92"/>
+      <c r="AU10" s="13">
         <v>71</v>
       </c>
-      <c r="AW10" s="14">
+      <c r="AV10" s="14">
         <v>80</v>
       </c>
-      <c r="AX10" s="15"/>
-      <c r="AY10" s="13">
+      <c r="AW10" s="15"/>
+      <c r="AX10" s="13">
         <v>71</v>
       </c>
-      <c r="AZ10" s="14">
+      <c r="AY10" s="14">
         <v>80</v>
       </c>
-      <c r="BA10" s="234"/>
+      <c r="AZ10" s="234"/>
+      <c r="BA10" s="97"/>
       <c r="BB10" s="97"/>
       <c r="BC10" s="97"/>
-      <c r="BD10" s="97"/>
-    </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A11" s="209"/>
       <c r="B11" s="108"/>
       <c r="C11" s="221">
@@ -14518,7 +14548,7 @@
       <c r="X11" s="14">
         <v>90</v>
       </c>
-      <c r="Y11" s="17"/>
+      <c r="Y11" s="246"/>
       <c r="Z11" s="149"/>
       <c r="AA11" s="187"/>
       <c r="AB11" s="163"/>
@@ -14531,35 +14561,34 @@
       <c r="AI11" s="112"/>
       <c r="AJ11" s="129"/>
       <c r="AK11" s="194"/>
-      <c r="AL11" s="195"/>
-      <c r="AM11" s="81"/>
-      <c r="AN11" s="216"/>
-      <c r="AO11" s="109"/>
-      <c r="AP11" s="214"/>
-      <c r="AQ11" s="92"/>
-      <c r="AR11" s="214"/>
-      <c r="AS11" s="92"/>
-      <c r="AT11" s="214"/>
-      <c r="AU11" s="92"/>
-      <c r="AV11" s="13">
+      <c r="AL11" s="81"/>
+      <c r="AM11" s="216"/>
+      <c r="AN11" s="109"/>
+      <c r="AO11" s="214"/>
+      <c r="AP11" s="92"/>
+      <c r="AQ11" s="214"/>
+      <c r="AR11" s="92"/>
+      <c r="AS11" s="214"/>
+      <c r="AT11" s="92"/>
+      <c r="AU11" s="13">
         <v>81</v>
       </c>
-      <c r="AW11" s="14">
+      <c r="AV11" s="14">
         <v>90</v>
       </c>
-      <c r="AX11" s="15"/>
-      <c r="AY11" s="13">
+      <c r="AW11" s="15"/>
+      <c r="AX11" s="13">
         <v>81</v>
       </c>
-      <c r="AZ11" s="14">
+      <c r="AY11" s="14">
         <v>90</v>
       </c>
-      <c r="BA11" s="234"/>
+      <c r="AZ11" s="234"/>
+      <c r="BA11" s="97"/>
       <c r="BB11" s="97"/>
       <c r="BC11" s="97"/>
-      <c r="BD11" s="97"/>
-    </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" s="209"/>
       <c r="B12" s="108"/>
       <c r="C12" s="221">
@@ -14604,7 +14633,7 @@
       <c r="X12" s="14">
         <v>100</v>
       </c>
-      <c r="Y12" s="17"/>
+      <c r="Y12" s="245"/>
       <c r="Z12" s="149"/>
       <c r="AA12" s="187"/>
       <c r="AB12" s="163"/>
@@ -14617,35 +14646,34 @@
       <c r="AI12" s="112"/>
       <c r="AJ12" s="129"/>
       <c r="AK12" s="194"/>
-      <c r="AL12" s="195"/>
-      <c r="AM12" s="81"/>
-      <c r="AN12" s="216"/>
-      <c r="AO12" s="109"/>
-      <c r="AP12" s="214"/>
-      <c r="AQ12" s="92"/>
-      <c r="AR12" s="214"/>
-      <c r="AS12" s="92"/>
-      <c r="AT12" s="214"/>
-      <c r="AU12" s="92"/>
-      <c r="AV12" s="13">
+      <c r="AL12" s="81"/>
+      <c r="AM12" s="216"/>
+      <c r="AN12" s="109"/>
+      <c r="AO12" s="214"/>
+      <c r="AP12" s="92"/>
+      <c r="AQ12" s="214"/>
+      <c r="AR12" s="92"/>
+      <c r="AS12" s="214"/>
+      <c r="AT12" s="92"/>
+      <c r="AU12" s="13">
         <v>91</v>
       </c>
-      <c r="AW12" s="14">
+      <c r="AV12" s="14">
         <v>100</v>
       </c>
-      <c r="AX12" s="15"/>
-      <c r="AY12" s="13">
+      <c r="AW12" s="15"/>
+      <c r="AX12" s="13">
         <v>91</v>
       </c>
-      <c r="AZ12" s="14">
+      <c r="AY12" s="14">
         <v>100</v>
       </c>
-      <c r="BA12" s="234"/>
+      <c r="AZ12" s="234"/>
+      <c r="BA12" s="97"/>
       <c r="BB12" s="97"/>
       <c r="BC12" s="97"/>
-      <c r="BD12" s="97"/>
-    </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" s="209"/>
       <c r="B13" s="108"/>
       <c r="C13" s="221">
@@ -14690,7 +14718,7 @@
       <c r="X13" s="14">
         <v>110</v>
       </c>
-      <c r="Y13" s="17"/>
+      <c r="Y13" s="245"/>
       <c r="Z13" s="149"/>
       <c r="AA13" s="187"/>
       <c r="AB13" s="163"/>
@@ -14703,35 +14731,34 @@
       <c r="AI13" s="134"/>
       <c r="AJ13" s="130"/>
       <c r="AK13" s="194"/>
-      <c r="AL13" s="195"/>
-      <c r="AM13" s="81"/>
-      <c r="AN13" s="216"/>
-      <c r="AO13" s="109"/>
-      <c r="AP13" s="214"/>
-      <c r="AQ13" s="92"/>
-      <c r="AR13" s="214"/>
-      <c r="AS13" s="92"/>
-      <c r="AT13" s="214"/>
-      <c r="AU13" s="92"/>
-      <c r="AV13" s="13">
+      <c r="AL13" s="81"/>
+      <c r="AM13" s="216"/>
+      <c r="AN13" s="109"/>
+      <c r="AO13" s="214"/>
+      <c r="AP13" s="92"/>
+      <c r="AQ13" s="214"/>
+      <c r="AR13" s="92"/>
+      <c r="AS13" s="214"/>
+      <c r="AT13" s="92"/>
+      <c r="AU13" s="13">
         <v>101</v>
       </c>
-      <c r="AW13" s="14">
+      <c r="AV13" s="14">
         <v>110</v>
       </c>
-      <c r="AX13" s="15"/>
-      <c r="AY13" s="13">
+      <c r="AW13" s="15"/>
+      <c r="AX13" s="13">
         <v>101</v>
       </c>
-      <c r="AZ13" s="14">
+      <c r="AY13" s="14">
         <v>110</v>
       </c>
-      <c r="BA13" s="234"/>
+      <c r="AZ13" s="234"/>
+      <c r="BA13" s="97"/>
       <c r="BB13" s="97"/>
       <c r="BC13" s="97"/>
-      <c r="BD13" s="97"/>
-    </row>
-    <row r="14" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="209"/>
       <c r="B14" s="108"/>
       <c r="C14" s="221">
@@ -14776,7 +14803,7 @@
       <c r="X14" s="14">
         <v>120</v>
       </c>
-      <c r="Y14" s="17"/>
+      <c r="Y14" s="245"/>
       <c r="Z14" s="152"/>
       <c r="AA14" s="188"/>
       <c r="AB14" s="163"/>
@@ -14795,35 +14822,34 @@
         <v>43</v>
       </c>
       <c r="AK14" s="194"/>
-      <c r="AL14" s="195"/>
-      <c r="AM14" s="81"/>
-      <c r="AN14" s="216"/>
-      <c r="AO14" s="109"/>
-      <c r="AP14" s="214"/>
-      <c r="AQ14" s="92"/>
-      <c r="AR14" s="214"/>
-      <c r="AS14" s="92"/>
-      <c r="AT14" s="214"/>
-      <c r="AU14" s="92"/>
-      <c r="AV14" s="13">
+      <c r="AL14" s="81"/>
+      <c r="AM14" s="216"/>
+      <c r="AN14" s="109"/>
+      <c r="AO14" s="214"/>
+      <c r="AP14" s="92"/>
+      <c r="AQ14" s="214"/>
+      <c r="AR14" s="92"/>
+      <c r="AS14" s="214"/>
+      <c r="AT14" s="92"/>
+      <c r="AU14" s="13">
         <v>111</v>
       </c>
-      <c r="AW14" s="14">
+      <c r="AV14" s="14">
         <v>120</v>
       </c>
-      <c r="AX14" s="15"/>
-      <c r="AY14" s="13">
+      <c r="AW14" s="15"/>
+      <c r="AX14" s="13">
         <v>111</v>
       </c>
-      <c r="AZ14" s="14">
+      <c r="AY14" s="14">
         <v>120</v>
       </c>
-      <c r="BA14" s="234"/>
+      <c r="AZ14" s="234"/>
+      <c r="BA14" s="97"/>
       <c r="BB14" s="97"/>
       <c r="BC14" s="97"/>
-      <c r="BD14" s="97"/>
-    </row>
-    <row r="15" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="209"/>
       <c r="B15" s="108"/>
       <c r="C15" s="221">
@@ -14868,7 +14894,7 @@
       <c r="X15" s="14">
         <v>130</v>
       </c>
-      <c r="Y15" s="17"/>
+      <c r="Y15" s="244"/>
       <c r="Z15" s="75">
         <v>127</v>
       </c>
@@ -14895,35 +14921,34 @@
         <v>44</v>
       </c>
       <c r="AK15" s="194"/>
-      <c r="AL15" s="195"/>
-      <c r="AM15" s="81"/>
-      <c r="AN15" s="216"/>
-      <c r="AO15" s="109"/>
-      <c r="AP15" s="214"/>
-      <c r="AQ15" s="92"/>
-      <c r="AR15" s="214"/>
-      <c r="AS15" s="92"/>
-      <c r="AT15" s="214"/>
-      <c r="AU15" s="92"/>
-      <c r="AV15" s="13">
+      <c r="AL15" s="81"/>
+      <c r="AM15" s="216"/>
+      <c r="AN15" s="109"/>
+      <c r="AO15" s="214"/>
+      <c r="AP15" s="92"/>
+      <c r="AQ15" s="214"/>
+      <c r="AR15" s="92"/>
+      <c r="AS15" s="214"/>
+      <c r="AT15" s="92"/>
+      <c r="AU15" s="13">
         <v>120.833333333333</v>
       </c>
-      <c r="AW15" s="14">
+      <c r="AV15" s="14">
         <v>130</v>
       </c>
-      <c r="AX15" s="15"/>
-      <c r="AY15" s="13">
+      <c r="AW15" s="15"/>
+      <c r="AX15" s="13">
         <v>120.833333333333</v>
       </c>
-      <c r="AZ15" s="14">
+      <c r="AY15" s="14">
         <v>130</v>
       </c>
-      <c r="BA15" s="234"/>
+      <c r="AZ15" s="234"/>
+      <c r="BA15" s="97"/>
       <c r="BB15" s="97"/>
       <c r="BC15" s="97"/>
-      <c r="BD15" s="97"/>
-    </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" s="209"/>
       <c r="B16" s="108"/>
       <c r="C16" s="221">
@@ -14968,7 +14993,7 @@
       <c r="X16" s="14">
         <v>140</v>
       </c>
-      <c r="Y16" s="17"/>
+      <c r="Y16" s="245"/>
       <c r="Z16" s="148"/>
       <c r="AA16" s="189" t="s">
         <v>108</v>
@@ -14987,35 +15012,34 @@
       <c r="AI16" s="112"/>
       <c r="AJ16" s="81"/>
       <c r="AK16" s="194"/>
-      <c r="AL16" s="195"/>
-      <c r="AM16" s="81"/>
-      <c r="AN16" s="216"/>
-      <c r="AO16" s="109"/>
-      <c r="AP16" s="214"/>
-      <c r="AQ16" s="92"/>
-      <c r="AR16" s="214"/>
-      <c r="AS16" s="92"/>
-      <c r="AT16" s="214"/>
-      <c r="AU16" s="92"/>
-      <c r="AV16" s="13">
+      <c r="AL16" s="81"/>
+      <c r="AM16" s="216"/>
+      <c r="AN16" s="109"/>
+      <c r="AO16" s="214"/>
+      <c r="AP16" s="92"/>
+      <c r="AQ16" s="214"/>
+      <c r="AR16" s="92"/>
+      <c r="AS16" s="214"/>
+      <c r="AT16" s="92"/>
+      <c r="AU16" s="13">
         <v>131</v>
       </c>
-      <c r="AW16" s="14">
+      <c r="AV16" s="14">
         <v>140</v>
       </c>
-      <c r="AX16" s="15"/>
-      <c r="AY16" s="13">
+      <c r="AW16" s="15"/>
+      <c r="AX16" s="13">
         <v>131</v>
       </c>
-      <c r="AZ16" s="14">
+      <c r="AY16" s="14">
         <v>140</v>
       </c>
-      <c r="BA16" s="234"/>
+      <c r="AZ16" s="234"/>
+      <c r="BA16" s="97"/>
       <c r="BB16" s="97"/>
       <c r="BC16" s="97"/>
-      <c r="BD16" s="97"/>
-    </row>
-    <row r="17" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="209"/>
       <c r="B17" s="108"/>
       <c r="C17" s="221">
@@ -15060,7 +15084,7 @@
       <c r="X17" s="14">
         <v>150</v>
       </c>
-      <c r="Y17" s="17"/>
+      <c r="Y17" s="246"/>
       <c r="Z17" s="149"/>
       <c r="AA17" s="190"/>
       <c r="AB17" s="185"/>
@@ -15073,35 +15097,34 @@
       <c r="AI17" s="112"/>
       <c r="AJ17" s="81"/>
       <c r="AK17" s="194"/>
-      <c r="AL17" s="195"/>
-      <c r="AM17" s="81"/>
-      <c r="AN17" s="217"/>
-      <c r="AO17" s="165"/>
-      <c r="AP17" s="214"/>
-      <c r="AQ17" s="92"/>
-      <c r="AR17" s="214"/>
-      <c r="AS17" s="92"/>
-      <c r="AT17" s="214"/>
-      <c r="AU17" s="92"/>
-      <c r="AV17" s="13">
+      <c r="AL17" s="81"/>
+      <c r="AM17" s="217"/>
+      <c r="AN17" s="165"/>
+      <c r="AO17" s="214"/>
+      <c r="AP17" s="92"/>
+      <c r="AQ17" s="214"/>
+      <c r="AR17" s="92"/>
+      <c r="AS17" s="214"/>
+      <c r="AT17" s="92"/>
+      <c r="AU17" s="13">
         <v>141</v>
       </c>
-      <c r="AW17" s="14">
+      <c r="AV17" s="14">
         <v>150</v>
       </c>
-      <c r="AX17" s="15"/>
-      <c r="AY17" s="13">
+      <c r="AW17" s="15"/>
+      <c r="AX17" s="13">
         <v>141</v>
       </c>
-      <c r="AZ17" s="14">
+      <c r="AY17" s="14">
         <v>150</v>
       </c>
-      <c r="BA17" s="234"/>
+      <c r="AZ17" s="234"/>
+      <c r="BA17" s="97"/>
       <c r="BB17" s="97"/>
       <c r="BC17" s="97"/>
-      <c r="BD17" s="97"/>
-    </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A18" s="209"/>
       <c r="B18" s="108"/>
       <c r="C18" s="221">
@@ -15162,7 +15185,7 @@
       <c r="X18" s="14">
         <v>160</v>
       </c>
-      <c r="Y18" s="17"/>
+      <c r="Y18" s="245"/>
       <c r="Z18" s="149"/>
       <c r="AA18" s="190"/>
       <c r="AB18" s="204" t="s">
@@ -15183,43 +15206,42 @@
       <c r="AI18" s="112"/>
       <c r="AJ18" s="81"/>
       <c r="AK18" s="194"/>
-      <c r="AL18" s="195"/>
-      <c r="AM18" s="81"/>
-      <c r="AN18" s="178" t="s">
+      <c r="AL18" s="81"/>
+      <c r="AM18" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="AO18" s="140"/>
-      <c r="AP18" s="178" t="s">
+      <c r="AN18" s="140"/>
+      <c r="AO18" s="178" t="s">
         <v>71</v>
       </c>
-      <c r="AQ18" s="140"/>
-      <c r="AR18" s="178" t="s">
+      <c r="AP18" s="140"/>
+      <c r="AQ18" s="178" t="s">
         <v>72</v>
       </c>
-      <c r="AS18" s="140"/>
-      <c r="AT18" s="178" t="s">
+      <c r="AR18" s="140"/>
+      <c r="AS18" s="178" t="s">
         <v>72</v>
       </c>
-      <c r="AU18" s="140"/>
-      <c r="AV18" s="13">
+      <c r="AT18" s="140"/>
+      <c r="AU18" s="13">
         <v>150.833333333333</v>
       </c>
-      <c r="AW18" s="14">
+      <c r="AV18" s="14">
         <v>160</v>
       </c>
-      <c r="AX18" s="15"/>
-      <c r="AY18" s="13">
+      <c r="AW18" s="15"/>
+      <c r="AX18" s="13">
         <v>150.833333333333</v>
       </c>
-      <c r="AZ18" s="14">
+      <c r="AY18" s="14">
         <v>160</v>
       </c>
-      <c r="BA18" s="234"/>
+      <c r="AZ18" s="234"/>
+      <c r="BA18" s="97"/>
       <c r="BB18" s="97"/>
       <c r="BC18" s="97"/>
-      <c r="BD18" s="97"/>
-    </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A19" s="209"/>
       <c r="B19" s="108"/>
       <c r="C19" s="221">
@@ -15264,7 +15286,7 @@
       <c r="X19" s="14">
         <v>170</v>
       </c>
-      <c r="Y19" s="17"/>
+      <c r="Y19" s="245"/>
       <c r="Z19" s="149"/>
       <c r="AA19" s="190"/>
       <c r="AB19" s="205"/>
@@ -15277,35 +15299,34 @@
       <c r="AI19" s="112"/>
       <c r="AJ19" s="81"/>
       <c r="AK19" s="194"/>
-      <c r="AL19" s="195"/>
-      <c r="AM19" s="81"/>
-      <c r="AN19" s="179"/>
-      <c r="AO19" s="142"/>
-      <c r="AP19" s="179"/>
-      <c r="AQ19" s="142"/>
-      <c r="AR19" s="179"/>
-      <c r="AS19" s="142"/>
-      <c r="AT19" s="179"/>
-      <c r="AU19" s="142"/>
-      <c r="AV19" s="13">
+      <c r="AL19" s="81"/>
+      <c r="AM19" s="179"/>
+      <c r="AN19" s="142"/>
+      <c r="AO19" s="179"/>
+      <c r="AP19" s="142"/>
+      <c r="AQ19" s="179"/>
+      <c r="AR19" s="142"/>
+      <c r="AS19" s="179"/>
+      <c r="AT19" s="142"/>
+      <c r="AU19" s="13">
         <v>161</v>
       </c>
-      <c r="AW19" s="14">
+      <c r="AV19" s="14">
         <v>170</v>
       </c>
-      <c r="AX19" s="15"/>
-      <c r="AY19" s="13">
+      <c r="AW19" s="15"/>
+      <c r="AX19" s="13">
         <v>161</v>
       </c>
-      <c r="AZ19" s="14">
+      <c r="AY19" s="14">
         <v>170</v>
       </c>
-      <c r="BA19" s="234"/>
+      <c r="AZ19" s="234"/>
+      <c r="BA19" s="97"/>
       <c r="BB19" s="97"/>
       <c r="BC19" s="97"/>
-      <c r="BD19" s="97"/>
-    </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" s="209"/>
       <c r="B20" s="108"/>
       <c r="C20" s="221">
@@ -15350,7 +15371,7 @@
       <c r="X20" s="14">
         <v>180</v>
       </c>
-      <c r="Y20" s="17"/>
+      <c r="Y20" s="245"/>
       <c r="Z20" s="149"/>
       <c r="AA20" s="190"/>
       <c r="AB20" s="205"/>
@@ -15363,35 +15384,34 @@
       <c r="AI20" s="112"/>
       <c r="AJ20" s="81"/>
       <c r="AK20" s="194"/>
-      <c r="AL20" s="195"/>
-      <c r="AM20" s="81"/>
-      <c r="AN20" s="179"/>
-      <c r="AO20" s="142"/>
-      <c r="AP20" s="179"/>
-      <c r="AQ20" s="142"/>
-      <c r="AR20" s="179"/>
-      <c r="AS20" s="142"/>
-      <c r="AT20" s="179"/>
-      <c r="AU20" s="142"/>
-      <c r="AV20" s="13">
+      <c r="AL20" s="81"/>
+      <c r="AM20" s="179"/>
+      <c r="AN20" s="142"/>
+      <c r="AO20" s="179"/>
+      <c r="AP20" s="142"/>
+      <c r="AQ20" s="179"/>
+      <c r="AR20" s="142"/>
+      <c r="AS20" s="179"/>
+      <c r="AT20" s="142"/>
+      <c r="AU20" s="13">
         <v>171</v>
       </c>
-      <c r="AW20" s="14">
+      <c r="AV20" s="14">
         <v>180</v>
       </c>
-      <c r="AX20" s="15"/>
-      <c r="AY20" s="13">
+      <c r="AW20" s="15"/>
+      <c r="AX20" s="13">
         <v>171</v>
       </c>
-      <c r="AZ20" s="14">
+      <c r="AY20" s="14">
         <v>180</v>
       </c>
-      <c r="BA20" s="234"/>
+      <c r="AZ20" s="234"/>
+      <c r="BA20" s="97"/>
       <c r="BB20" s="97"/>
       <c r="BC20" s="97"/>
-      <c r="BD20" s="97"/>
-    </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A21" s="209"/>
       <c r="B21" s="108"/>
       <c r="C21" s="221">
@@ -15449,35 +15469,34 @@
       <c r="AI21" s="112"/>
       <c r="AJ21" s="81"/>
       <c r="AK21" s="194"/>
-      <c r="AL21" s="195"/>
-      <c r="AM21" s="81"/>
-      <c r="AN21" s="179"/>
-      <c r="AO21" s="142"/>
-      <c r="AP21" s="179"/>
-      <c r="AQ21" s="142"/>
-      <c r="AR21" s="179"/>
-      <c r="AS21" s="142"/>
-      <c r="AT21" s="179"/>
-      <c r="AU21" s="142"/>
-      <c r="AV21" s="13">
+      <c r="AL21" s="81"/>
+      <c r="AM21" s="179"/>
+      <c r="AN21" s="142"/>
+      <c r="AO21" s="179"/>
+      <c r="AP21" s="142"/>
+      <c r="AQ21" s="179"/>
+      <c r="AR21" s="142"/>
+      <c r="AS21" s="179"/>
+      <c r="AT21" s="142"/>
+      <c r="AU21" s="13">
         <v>181</v>
       </c>
-      <c r="AW21" s="14">
+      <c r="AV21" s="14">
         <v>190</v>
       </c>
-      <c r="AX21" s="15"/>
-      <c r="AY21" s="13">
+      <c r="AW21" s="15"/>
+      <c r="AX21" s="13">
         <v>181</v>
       </c>
-      <c r="AZ21" s="14">
+      <c r="AY21" s="14">
         <v>190</v>
       </c>
-      <c r="BA21" s="234"/>
+      <c r="AZ21" s="234"/>
+      <c r="BA21" s="97"/>
       <c r="BB21" s="97"/>
       <c r="BC21" s="97"/>
-      <c r="BD21" s="97"/>
-    </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A22" s="209"/>
       <c r="B22" s="108"/>
       <c r="C22" s="221">
@@ -15535,35 +15554,34 @@
       <c r="AI22" s="134"/>
       <c r="AJ22" s="135"/>
       <c r="AK22" s="194"/>
-      <c r="AL22" s="195"/>
-      <c r="AM22" s="81"/>
-      <c r="AN22" s="179"/>
-      <c r="AO22" s="142"/>
-      <c r="AP22" s="179"/>
-      <c r="AQ22" s="142"/>
-      <c r="AR22" s="179"/>
-      <c r="AS22" s="142"/>
-      <c r="AT22" s="179"/>
-      <c r="AU22" s="142"/>
-      <c r="AV22" s="13">
+      <c r="AL22" s="81"/>
+      <c r="AM22" s="179"/>
+      <c r="AN22" s="142"/>
+      <c r="AO22" s="179"/>
+      <c r="AP22" s="142"/>
+      <c r="AQ22" s="179"/>
+      <c r="AR22" s="142"/>
+      <c r="AS22" s="179"/>
+      <c r="AT22" s="142"/>
+      <c r="AU22" s="13">
         <v>191</v>
       </c>
-      <c r="AW22" s="14">
+      <c r="AV22" s="14">
         <v>200</v>
       </c>
-      <c r="AX22" s="15"/>
-      <c r="AY22" s="13">
+      <c r="AW22" s="15"/>
+      <c r="AX22" s="13">
         <v>191</v>
       </c>
-      <c r="AZ22" s="14">
+      <c r="AY22" s="14">
         <v>200</v>
       </c>
-      <c r="BA22" s="234"/>
+      <c r="AZ22" s="234"/>
+      <c r="BA22" s="97"/>
       <c r="BB22" s="97"/>
       <c r="BC22" s="97"/>
-      <c r="BD22" s="97"/>
-    </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A23" s="209"/>
       <c r="B23" s="108"/>
       <c r="C23" s="221">
@@ -15627,35 +15645,34 @@
         <v>45</v>
       </c>
       <c r="AK23" s="194"/>
-      <c r="AL23" s="195"/>
-      <c r="AM23" s="81"/>
-      <c r="AN23" s="179"/>
-      <c r="AO23" s="142"/>
-      <c r="AP23" s="179"/>
-      <c r="AQ23" s="142"/>
-      <c r="AR23" s="179"/>
-      <c r="AS23" s="142"/>
-      <c r="AT23" s="179"/>
-      <c r="AU23" s="142"/>
-      <c r="AV23" s="13">
+      <c r="AL23" s="81"/>
+      <c r="AM23" s="179"/>
+      <c r="AN23" s="142"/>
+      <c r="AO23" s="179"/>
+      <c r="AP23" s="142"/>
+      <c r="AQ23" s="179"/>
+      <c r="AR23" s="142"/>
+      <c r="AS23" s="179"/>
+      <c r="AT23" s="142"/>
+      <c r="AU23" s="13">
         <v>201</v>
       </c>
-      <c r="AW23" s="14">
+      <c r="AV23" s="14">
         <v>210</v>
       </c>
-      <c r="AX23" s="15"/>
-      <c r="AY23" s="13">
+      <c r="AW23" s="15"/>
+      <c r="AX23" s="13">
         <v>201</v>
       </c>
-      <c r="AZ23" s="14">
+      <c r="AY23" s="14">
         <v>210</v>
       </c>
-      <c r="BA23" s="234"/>
+      <c r="AZ23" s="234"/>
+      <c r="BA23" s="97"/>
       <c r="BB23" s="97"/>
       <c r="BC23" s="97"/>
-      <c r="BD23" s="97"/>
-    </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A24" s="209"/>
       <c r="B24" s="108"/>
       <c r="C24" s="221">
@@ -15713,35 +15730,34 @@
       <c r="AI24" s="112"/>
       <c r="AJ24" s="81"/>
       <c r="AK24" s="194"/>
-      <c r="AL24" s="195"/>
-      <c r="AM24" s="81"/>
-      <c r="AN24" s="179"/>
-      <c r="AO24" s="142"/>
-      <c r="AP24" s="179"/>
-      <c r="AQ24" s="142"/>
-      <c r="AR24" s="179"/>
-      <c r="AS24" s="142"/>
-      <c r="AT24" s="179"/>
-      <c r="AU24" s="142"/>
-      <c r="AV24" s="13">
+      <c r="AL24" s="81"/>
+      <c r="AM24" s="179"/>
+      <c r="AN24" s="142"/>
+      <c r="AO24" s="179"/>
+      <c r="AP24" s="142"/>
+      <c r="AQ24" s="179"/>
+      <c r="AR24" s="142"/>
+      <c r="AS24" s="179"/>
+      <c r="AT24" s="142"/>
+      <c r="AU24" s="13">
         <v>210</v>
       </c>
-      <c r="AW24" s="14">
+      <c r="AV24" s="14">
         <v>220</v>
       </c>
-      <c r="AX24" s="15"/>
-      <c r="AY24" s="13">
+      <c r="AW24" s="15"/>
+      <c r="AX24" s="13">
         <v>210</v>
       </c>
-      <c r="AZ24" s="14">
+      <c r="AY24" s="14">
         <v>220</v>
       </c>
-      <c r="BA24" s="234"/>
+      <c r="AZ24" s="234"/>
+      <c r="BA24" s="97"/>
       <c r="BB24" s="97"/>
       <c r="BC24" s="97"/>
-      <c r="BD24" s="97"/>
-    </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A25" s="209"/>
       <c r="B25" s="108"/>
       <c r="C25" s="221">
@@ -15799,35 +15815,34 @@
       <c r="AI25" s="112"/>
       <c r="AJ25" s="81"/>
       <c r="AK25" s="194"/>
-      <c r="AL25" s="195"/>
-      <c r="AM25" s="81"/>
-      <c r="AN25" s="179"/>
-      <c r="AO25" s="142"/>
-      <c r="AP25" s="179"/>
-      <c r="AQ25" s="142"/>
-      <c r="AR25" s="179"/>
-      <c r="AS25" s="142"/>
-      <c r="AT25" s="179"/>
-      <c r="AU25" s="142"/>
-      <c r="AV25" s="13">
+      <c r="AL25" s="81"/>
+      <c r="AM25" s="179"/>
+      <c r="AN25" s="142"/>
+      <c r="AO25" s="179"/>
+      <c r="AP25" s="142"/>
+      <c r="AQ25" s="179"/>
+      <c r="AR25" s="142"/>
+      <c r="AS25" s="179"/>
+      <c r="AT25" s="142"/>
+      <c r="AU25" s="13">
         <v>221</v>
       </c>
-      <c r="AW25" s="14">
+      <c r="AV25" s="14">
         <v>230</v>
       </c>
-      <c r="AX25" s="15"/>
-      <c r="AY25" s="13">
+      <c r="AW25" s="15"/>
+      <c r="AX25" s="13">
         <v>221</v>
       </c>
-      <c r="AZ25" s="14">
+      <c r="AY25" s="14">
         <v>230</v>
       </c>
-      <c r="BA25" s="234"/>
+      <c r="AZ25" s="234"/>
+      <c r="BA25" s="97"/>
       <c r="BB25" s="97"/>
       <c r="BC25" s="97"/>
-      <c r="BD25" s="97"/>
-    </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A26" s="209"/>
       <c r="B26" s="108"/>
       <c r="C26" s="221">
@@ -15887,35 +15902,34 @@
       <c r="AI26" s="112"/>
       <c r="AJ26" s="81"/>
       <c r="AK26" s="194"/>
-      <c r="AL26" s="195"/>
-      <c r="AM26" s="81"/>
-      <c r="AN26" s="179"/>
-      <c r="AO26" s="142"/>
-      <c r="AP26" s="179"/>
-      <c r="AQ26" s="142"/>
-      <c r="AR26" s="179"/>
-      <c r="AS26" s="142"/>
-      <c r="AT26" s="179"/>
-      <c r="AU26" s="142"/>
-      <c r="AV26" s="13">
+      <c r="AL26" s="81"/>
+      <c r="AM26" s="179"/>
+      <c r="AN26" s="142"/>
+      <c r="AO26" s="179"/>
+      <c r="AP26" s="142"/>
+      <c r="AQ26" s="179"/>
+      <c r="AR26" s="142"/>
+      <c r="AS26" s="179"/>
+      <c r="AT26" s="142"/>
+      <c r="AU26" s="13">
         <v>231</v>
       </c>
-      <c r="AW26" s="14">
+      <c r="AV26" s="14">
         <v>240</v>
       </c>
-      <c r="AX26" s="15"/>
-      <c r="AY26" s="13">
+      <c r="AW26" s="15"/>
+      <c r="AX26" s="13">
         <v>231</v>
       </c>
-      <c r="AZ26" s="14">
+      <c r="AY26" s="14">
         <v>240</v>
       </c>
-      <c r="BA26" s="234"/>
+      <c r="AZ26" s="234"/>
+      <c r="BA26" s="97"/>
       <c r="BB26" s="97"/>
       <c r="BC26" s="97"/>
-      <c r="BD26" s="97"/>
-    </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A27" s="209"/>
       <c r="B27" s="108"/>
       <c r="C27" s="221">
@@ -15975,35 +15989,34 @@
       <c r="AI27" s="112"/>
       <c r="AJ27" s="81"/>
       <c r="AK27" s="194"/>
-      <c r="AL27" s="195"/>
-      <c r="AM27" s="81"/>
-      <c r="AN27" s="179"/>
-      <c r="AO27" s="142"/>
-      <c r="AP27" s="179"/>
-      <c r="AQ27" s="142"/>
-      <c r="AR27" s="179"/>
-      <c r="AS27" s="142"/>
-      <c r="AT27" s="179"/>
-      <c r="AU27" s="142"/>
-      <c r="AV27" s="13">
+      <c r="AL27" s="81"/>
+      <c r="AM27" s="179"/>
+      <c r="AN27" s="142"/>
+      <c r="AO27" s="179"/>
+      <c r="AP27" s="142"/>
+      <c r="AQ27" s="179"/>
+      <c r="AR27" s="142"/>
+      <c r="AS27" s="179"/>
+      <c r="AT27" s="142"/>
+      <c r="AU27" s="13">
         <v>241</v>
       </c>
-      <c r="AW27" s="14">
+      <c r="AV27" s="14">
         <v>250</v>
       </c>
-      <c r="AX27" s="15"/>
-      <c r="AY27" s="13">
+      <c r="AW27" s="15"/>
+      <c r="AX27" s="13">
         <v>241</v>
       </c>
-      <c r="AZ27" s="14">
+      <c r="AY27" s="14">
         <v>250</v>
       </c>
-      <c r="BA27" s="234"/>
+      <c r="AZ27" s="234"/>
+      <c r="BA27" s="97"/>
       <c r="BB27" s="97"/>
       <c r="BC27" s="97"/>
-      <c r="BD27" s="97"/>
-    </row>
-    <row r="28" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="210"/>
       <c r="B28" s="211"/>
       <c r="C28" s="225">
@@ -16063,37 +16076,36 @@
       <c r="AI28" s="112"/>
       <c r="AJ28" s="81"/>
       <c r="AK28" s="196"/>
-      <c r="AL28" s="197"/>
-      <c r="AM28" s="82"/>
-      <c r="AN28" s="180"/>
-      <c r="AO28" s="144"/>
-      <c r="AP28" s="180"/>
-      <c r="AQ28" s="144"/>
-      <c r="AR28" s="180"/>
-      <c r="AS28" s="144"/>
-      <c r="AT28" s="180"/>
-      <c r="AU28" s="144"/>
-      <c r="AV28" s="59">
+      <c r="AL28" s="82"/>
+      <c r="AM28" s="180"/>
+      <c r="AN28" s="144"/>
+      <c r="AO28" s="180"/>
+      <c r="AP28" s="144"/>
+      <c r="AQ28" s="180"/>
+      <c r="AR28" s="144"/>
+      <c r="AS28" s="180"/>
+      <c r="AT28" s="144"/>
+      <c r="AU28" s="59">
         <v>251</v>
       </c>
-      <c r="AW28" s="53">
+      <c r="AV28" s="53">
         <v>255</v>
       </c>
-      <c r="AX28" s="54"/>
-      <c r="AY28" s="235">
+      <c r="AW28" s="54"/>
+      <c r="AX28" s="235">
         <v>251</v>
       </c>
-      <c r="AZ28" s="236">
+      <c r="AY28" s="236">
         <v>255</v>
       </c>
-      <c r="BA28" s="237" t="s">
+      <c r="AZ28" s="237" t="s">
         <v>118</v>
       </c>
+      <c r="BA28" s="98"/>
       <c r="BB28" s="98"/>
       <c r="BC28" s="98"/>
-      <c r="BD28" s="98"/>
-    </row>
-    <row r="29" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="58" t="s">
         <v>85</v>
       </c>
@@ -16153,45 +16165,53 @@
       <c r="AK29" s="166">
         <v>8</v>
       </c>
-      <c r="AL29" s="167"/>
-      <c r="AM29" s="168"/>
-      <c r="AN29" s="174">
+      <c r="AL29" s="168"/>
+      <c r="AM29" s="174">
         <v>9</v>
       </c>
-      <c r="AO29" s="207"/>
-      <c r="AP29" s="172">
+      <c r="AN29" s="207"/>
+      <c r="AO29" s="172">
         <v>10</v>
       </c>
-      <c r="AQ29" s="173"/>
-      <c r="AR29" s="172">
+      <c r="AP29" s="173"/>
+      <c r="AQ29" s="172">
         <v>11</v>
       </c>
-      <c r="AS29" s="173"/>
-      <c r="AT29" s="172">
+      <c r="AR29" s="173"/>
+      <c r="AS29" s="172">
         <v>12</v>
       </c>
-      <c r="AU29" s="173"/>
-      <c r="AV29" s="228">
+      <c r="AT29" s="173"/>
+      <c r="AU29" s="228">
         <v>13</v>
       </c>
-      <c r="AW29" s="229"/>
-      <c r="AX29" s="230"/>
-      <c r="AY29" s="228">
+      <c r="AV29" s="229"/>
+      <c r="AW29" s="230"/>
+      <c r="AX29" s="228">
         <v>14</v>
       </c>
-      <c r="AZ29" s="229"/>
-      <c r="BA29" s="230"/>
+      <c r="AY29" s="229"/>
+      <c r="AZ29" s="230"/>
+      <c r="BA29" s="231">
+        <v>15</v>
+      </c>
       <c r="BB29" s="231">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BC29" s="231">
-        <v>16</v>
-      </c>
-      <c r="BD29" s="231">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="23:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="Y30" s="247"/>
+    </row>
+    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="Y31" s="248"/>
+    </row>
+    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="Y32" s="248"/>
+    </row>
+    <row r="33" spans="23:39" x14ac:dyDescent="0.25">
       <c r="W33" s="212" t="s">
         <v>95</v>
       </c>
@@ -16211,9 +16231,8 @@
       <c r="AK33" s="212"/>
       <c r="AL33" s="212"/>
       <c r="AM33" s="212"/>
-      <c r="AN33" s="212"/>
-    </row>
-    <row r="34" spans="23:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="23:39" x14ac:dyDescent="0.25">
       <c r="W34" s="212"/>
       <c r="X34" s="212"/>
       <c r="Y34" s="212"/>
@@ -16231,9 +16250,8 @@
       <c r="AK34" s="212"/>
       <c r="AL34" s="212"/>
       <c r="AM34" s="212"/>
-      <c r="AN34" s="212"/>
-    </row>
-    <row r="35" spans="23:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="23:39" x14ac:dyDescent="0.25">
       <c r="W35" s="212"/>
       <c r="X35" s="212"/>
       <c r="Y35" s="212"/>
@@ -16251,9 +16269,8 @@
       <c r="AK35" s="212"/>
       <c r="AL35" s="212"/>
       <c r="AM35" s="212"/>
-      <c r="AN35" s="212"/>
-    </row>
-    <row r="36" spans="23:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="23:39" x14ac:dyDescent="0.25">
       <c r="W36" s="212"/>
       <c r="X36" s="212"/>
       <c r="Y36" s="212"/>
@@ -16271,9 +16288,8 @@
       <c r="AK36" s="212"/>
       <c r="AL36" s="212"/>
       <c r="AM36" s="212"/>
-      <c r="AN36" s="212"/>
-    </row>
-    <row r="37" spans="23:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="23:39" x14ac:dyDescent="0.25">
       <c r="W37" s="212"/>
       <c r="X37" s="212"/>
       <c r="Y37" s="212"/>
@@ -16291,20 +16307,19 @@
       <c r="AK37" s="212"/>
       <c r="AL37" s="212"/>
       <c r="AM37" s="212"/>
-      <c r="AN37" s="212"/>
     </row>
   </sheetData>
   <mergeCells count="105">
-    <mergeCell ref="AT29:AU29"/>
-    <mergeCell ref="AV29:AX29"/>
-    <mergeCell ref="AY29:BA29"/>
-    <mergeCell ref="W33:AN37"/>
+    <mergeCell ref="AS29:AT29"/>
+    <mergeCell ref="AU29:AW29"/>
+    <mergeCell ref="AX29:AZ29"/>
+    <mergeCell ref="W33:AM37"/>
     <mergeCell ref="AD29:AG29"/>
     <mergeCell ref="AH29:AJ29"/>
-    <mergeCell ref="AK29:AM29"/>
-    <mergeCell ref="AN29:AO29"/>
-    <mergeCell ref="AP29:AQ29"/>
-    <mergeCell ref="AR29:AS29"/>
+    <mergeCell ref="AK29:AL29"/>
+    <mergeCell ref="AM29:AN29"/>
+    <mergeCell ref="AO29:AP29"/>
+    <mergeCell ref="AQ29:AR29"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="H29:L29"/>
     <mergeCell ref="M29:Q29"/>
@@ -16327,8 +16342,8 @@
     <mergeCell ref="L18:L28"/>
     <mergeCell ref="P18:P28"/>
     <mergeCell ref="Q18:Q28"/>
+    <mergeCell ref="BB3:BB28"/>
     <mergeCell ref="BC3:BC28"/>
-    <mergeCell ref="BD3:BD28"/>
     <mergeCell ref="Z4:Z14"/>
     <mergeCell ref="AD4:AD14"/>
     <mergeCell ref="AH6:AH13"/>
@@ -16337,26 +16352,26 @@
     <mergeCell ref="AH15:AH22"/>
     <mergeCell ref="AI15:AI22"/>
     <mergeCell ref="AJ15:AJ22"/>
+    <mergeCell ref="AP3:AP17"/>
     <mergeCell ref="AQ3:AQ17"/>
     <mergeCell ref="AR3:AR17"/>
     <mergeCell ref="AS3:AS17"/>
     <mergeCell ref="AT3:AT17"/>
-    <mergeCell ref="AU3:AU17"/>
-    <mergeCell ref="BB3:BB28"/>
-    <mergeCell ref="AP18:AQ28"/>
-    <mergeCell ref="AR18:AS28"/>
-    <mergeCell ref="AT18:AU28"/>
+    <mergeCell ref="BA3:BA28"/>
+    <mergeCell ref="AO18:AP28"/>
+    <mergeCell ref="AQ18:AR28"/>
+    <mergeCell ref="AS18:AT28"/>
     <mergeCell ref="AF3:AG17"/>
-    <mergeCell ref="AK3:AL28"/>
-    <mergeCell ref="AM3:AM28"/>
+    <mergeCell ref="AK3:AK28"/>
+    <mergeCell ref="AL3:AL28"/>
+    <mergeCell ref="AM3:AM17"/>
     <mergeCell ref="AN3:AN17"/>
     <mergeCell ref="AO3:AO17"/>
-    <mergeCell ref="AP3:AP17"/>
-    <mergeCell ref="AN18:AO28"/>
+    <mergeCell ref="AM18:AN28"/>
     <mergeCell ref="AH23:AH28"/>
     <mergeCell ref="AI23:AI28"/>
     <mergeCell ref="AJ23:AJ28"/>
-    <mergeCell ref="AY2:BA2"/>
+    <mergeCell ref="AX2:AZ2"/>
     <mergeCell ref="A3:A28"/>
     <mergeCell ref="B3:B28"/>
     <mergeCell ref="F3:G17"/>
@@ -16366,21 +16381,21 @@
     <mergeCell ref="AA3:AA14"/>
     <mergeCell ref="AB3:AC17"/>
     <mergeCell ref="AE3:AE14"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AX2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU2:AW2"/>
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AV1:AX1"/>
-    <mergeCell ref="AY1:BA1"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="AU1:AW1"/>
+    <mergeCell ref="AX1:AZ1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:J2"/>
@@ -16390,10 +16405,2837 @@
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="AH1:AJ1"/>
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FD46E4-3FD3-4779-A262-B30143228211}">
+  <dimension ref="A1:AZ37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AX37" sqref="AX37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="2"/>
+    <col min="8" max="9" width="6.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1"/>
+    <col min="13" max="14" width="6.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="1"/>
+    <col min="18" max="19" width="6.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="1"/>
+    <col min="23" max="24" width="6.7109375" customWidth="1"/>
+    <col min="34" max="35" width="6.7109375" customWidth="1"/>
+    <col min="47" max="48" width="6.7109375" style="2" customWidth="1"/>
+    <col min="49" max="49" width="16.7109375" style="232" customWidth="1"/>
+    <col min="50" max="52" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="181">
+        <v>2</v>
+      </c>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="181">
+        <v>3</v>
+      </c>
+      <c r="I1" s="182"/>
+      <c r="J1" s="182"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="181">
+        <v>4</v>
+      </c>
+      <c r="N1" s="182"/>
+      <c r="O1" s="182"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="181">
+        <v>5</v>
+      </c>
+      <c r="S1" s="182"/>
+      <c r="T1" s="182"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="83">
+        <v>6</v>
+      </c>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="181">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="182"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="104"/>
+      <c r="AD1" s="103">
+        <v>8</v>
+      </c>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="104"/>
+      <c r="AH1" s="83">
+        <v>9</v>
+      </c>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="84"/>
+      <c r="AK1" s="83">
+        <v>10</v>
+      </c>
+      <c r="AL1" s="84"/>
+      <c r="AM1" s="103">
+        <v>11</v>
+      </c>
+      <c r="AN1" s="104"/>
+      <c r="AO1" s="103">
+        <v>12</v>
+      </c>
+      <c r="AP1" s="104"/>
+      <c r="AQ1" s="103">
+        <v>13</v>
+      </c>
+      <c r="AR1" s="104"/>
+      <c r="AS1" s="103">
+        <v>14</v>
+      </c>
+      <c r="AT1" s="104"/>
+      <c r="AU1" s="83">
+        <v>15</v>
+      </c>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="84"/>
+      <c r="AX1" s="3">
+        <v>16</v>
+      </c>
+      <c r="AY1" s="3">
+        <v>17</v>
+      </c>
+      <c r="AZ1" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="156" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="157"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="101" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="100"/>
+      <c r="H2" s="156" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="157"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="100"/>
+      <c r="M2" s="156" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="157"/>
+      <c r="O2" s="158"/>
+      <c r="P2" s="101" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="156" t="s">
+        <v>106</v>
+      </c>
+      <c r="S2" s="157"/>
+      <c r="T2" s="158"/>
+      <c r="U2" s="101" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="100"/>
+      <c r="W2" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" s="87"/>
+      <c r="Y2" s="88"/>
+      <c r="Z2" s="156" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA2" s="158"/>
+      <c r="AB2" s="101" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="100"/>
+      <c r="AD2" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" s="101"/>
+      <c r="AF2" s="101"/>
+      <c r="AG2" s="100"/>
+      <c r="AH2" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI2" s="87"/>
+      <c r="AJ2" s="90"/>
+      <c r="AK2" s="89" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL2" s="90"/>
+      <c r="AM2" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN2" s="100"/>
+      <c r="AO2" s="99" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP2" s="100"/>
+      <c r="AQ2" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR2" s="100"/>
+      <c r="AS2" s="99" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT2" s="100"/>
+      <c r="AU2" s="89" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV2" s="87"/>
+      <c r="AW2" s="90"/>
+      <c r="AX2" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY2" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ2" s="51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A3" s="208"/>
+      <c r="B3" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="218">
+        <v>0</v>
+      </c>
+      <c r="D3" s="219">
+        <v>10</v>
+      </c>
+      <c r="E3" s="220" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="162" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="107"/>
+      <c r="H3" s="218">
+        <v>0</v>
+      </c>
+      <c r="I3" s="219">
+        <v>10</v>
+      </c>
+      <c r="J3" s="220" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="162" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="107"/>
+      <c r="M3" s="218">
+        <v>0</v>
+      </c>
+      <c r="N3" s="219">
+        <v>10</v>
+      </c>
+      <c r="O3" s="220" t="s">
+        <v>97</v>
+      </c>
+      <c r="P3" s="162" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="107"/>
+      <c r="R3" s="218">
+        <v>0</v>
+      </c>
+      <c r="S3" s="219">
+        <v>10</v>
+      </c>
+      <c r="T3" s="220" t="s">
+        <v>97</v>
+      </c>
+      <c r="U3" s="162" t="s">
+        <v>15</v>
+      </c>
+      <c r="V3" s="107"/>
+      <c r="W3" s="8">
+        <v>0</v>
+      </c>
+      <c r="X3" s="9">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z3" s="74">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="186" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB3" s="162" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="107"/>
+      <c r="AD3" s="74">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="186" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF3" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG3" s="107"/>
+      <c r="AH3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="9">
+        <v>10</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK3" s="192" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL3" s="114" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM3" s="215" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN3" s="107" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO3" s="213" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP3" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ3" s="213" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR3" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS3" s="213" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT3" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="9">
+        <v>10</v>
+      </c>
+      <c r="AW3" s="233" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX3" s="96" t="s">
+        <v>93</v>
+      </c>
+      <c r="AY3" s="96" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ3" s="96" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A4" s="209"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="221">
+        <v>11</v>
+      </c>
+      <c r="D4" s="222">
+        <v>20</v>
+      </c>
+      <c r="E4" s="223" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="163"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="221">
+        <v>11</v>
+      </c>
+      <c r="I4" s="222">
+        <v>20</v>
+      </c>
+      <c r="J4" s="223" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="163"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="221">
+        <v>11</v>
+      </c>
+      <c r="N4" s="222">
+        <v>20</v>
+      </c>
+      <c r="O4" s="223" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" s="163"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="221">
+        <v>11</v>
+      </c>
+      <c r="S4" s="222">
+        <v>20</v>
+      </c>
+      <c r="T4" s="223" t="s">
+        <v>98</v>
+      </c>
+      <c r="U4" s="163"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="13">
+        <v>11</v>
+      </c>
+      <c r="X4" s="14">
+        <v>20</v>
+      </c>
+      <c r="Y4" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z4" s="151"/>
+      <c r="AA4" s="187"/>
+      <c r="AB4" s="163"/>
+      <c r="AC4" s="109"/>
+      <c r="AD4" s="151"/>
+      <c r="AE4" s="187"/>
+      <c r="AF4" s="108"/>
+      <c r="AG4" s="109"/>
+      <c r="AH4" s="13">
+        <v>11</v>
+      </c>
+      <c r="AI4" s="14">
+        <v>20</v>
+      </c>
+      <c r="AJ4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK4" s="194"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="216"/>
+      <c r="AN4" s="109"/>
+      <c r="AO4" s="214"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="214"/>
+      <c r="AR4" s="92"/>
+      <c r="AS4" s="214"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="13">
+        <v>11</v>
+      </c>
+      <c r="AV4" s="14">
+        <v>20</v>
+      </c>
+      <c r="AW4" s="234" t="s">
+        <v>74</v>
+      </c>
+      <c r="AX4" s="97"/>
+      <c r="AY4" s="97"/>
+      <c r="AZ4" s="97"/>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A5" s="209"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="221">
+        <v>21</v>
+      </c>
+      <c r="D5" s="222">
+        <v>30</v>
+      </c>
+      <c r="E5" s="223" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="163"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="221">
+        <v>21</v>
+      </c>
+      <c r="I5" s="222">
+        <v>30</v>
+      </c>
+      <c r="J5" s="223" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" s="163"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="221">
+        <v>21</v>
+      </c>
+      <c r="N5" s="222">
+        <v>30</v>
+      </c>
+      <c r="O5" s="223" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" s="163"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="221">
+        <v>21</v>
+      </c>
+      <c r="S5" s="222">
+        <v>30</v>
+      </c>
+      <c r="T5" s="223" t="s">
+        <v>99</v>
+      </c>
+      <c r="U5" s="163"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="13">
+        <v>21</v>
+      </c>
+      <c r="X5" s="14">
+        <v>30</v>
+      </c>
+      <c r="Y5" s="70">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="Z5" s="149"/>
+      <c r="AA5" s="187"/>
+      <c r="AB5" s="163"/>
+      <c r="AC5" s="109"/>
+      <c r="AD5" s="149"/>
+      <c r="AE5" s="187"/>
+      <c r="AF5" s="108"/>
+      <c r="AG5" s="109"/>
+      <c r="AH5" s="13">
+        <v>21</v>
+      </c>
+      <c r="AI5" s="14">
+        <v>30</v>
+      </c>
+      <c r="AJ5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK5" s="194"/>
+      <c r="AL5" s="81"/>
+      <c r="AM5" s="216"/>
+      <c r="AN5" s="109"/>
+      <c r="AO5" s="214"/>
+      <c r="AP5" s="92"/>
+      <c r="AQ5" s="214"/>
+      <c r="AR5" s="92"/>
+      <c r="AS5" s="214"/>
+      <c r="AT5" s="92"/>
+      <c r="AU5" s="13">
+        <v>21</v>
+      </c>
+      <c r="AV5" s="14">
+        <v>30</v>
+      </c>
+      <c r="AW5" s="234" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX5" s="97"/>
+      <c r="AY5" s="97"/>
+      <c r="AZ5" s="97"/>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A6" s="209"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="221">
+        <v>31</v>
+      </c>
+      <c r="D6" s="222">
+        <v>40</v>
+      </c>
+      <c r="E6" s="223" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="163"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="221">
+        <v>31</v>
+      </c>
+      <c r="I6" s="222">
+        <v>40</v>
+      </c>
+      <c r="J6" s="223" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" s="163"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="221">
+        <v>31</v>
+      </c>
+      <c r="N6" s="222">
+        <v>40</v>
+      </c>
+      <c r="O6" s="223" t="s">
+        <v>100</v>
+      </c>
+      <c r="P6" s="163"/>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="221">
+        <v>31</v>
+      </c>
+      <c r="S6" s="222">
+        <v>40</v>
+      </c>
+      <c r="T6" s="223" t="s">
+        <v>100</v>
+      </c>
+      <c r="U6" s="163"/>
+      <c r="V6" s="109"/>
+      <c r="W6" s="13">
+        <v>31</v>
+      </c>
+      <c r="X6" s="14">
+        <v>40</v>
+      </c>
+      <c r="Y6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="187"/>
+      <c r="AB6" s="163"/>
+      <c r="AC6" s="109"/>
+      <c r="AD6" s="149"/>
+      <c r="AE6" s="187"/>
+      <c r="AF6" s="108"/>
+      <c r="AG6" s="109"/>
+      <c r="AH6" s="131">
+        <v>31</v>
+      </c>
+      <c r="AI6" s="133">
+        <v>110</v>
+      </c>
+      <c r="AJ6" s="128" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK6" s="194"/>
+      <c r="AL6" s="81"/>
+      <c r="AM6" s="216"/>
+      <c r="AN6" s="109"/>
+      <c r="AO6" s="214"/>
+      <c r="AP6" s="92"/>
+      <c r="AQ6" s="214"/>
+      <c r="AR6" s="92"/>
+      <c r="AS6" s="214"/>
+      <c r="AT6" s="92"/>
+      <c r="AU6" s="13">
+        <v>31</v>
+      </c>
+      <c r="AV6" s="14">
+        <v>40</v>
+      </c>
+      <c r="AW6" s="234" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX6" s="97"/>
+      <c r="AY6" s="97"/>
+      <c r="AZ6" s="97"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A7" s="209"/>
+      <c r="B7" s="108"/>
+      <c r="C7" s="221">
+        <v>41</v>
+      </c>
+      <c r="D7" s="222">
+        <v>50</v>
+      </c>
+      <c r="E7" s="223" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="163"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="221">
+        <v>41</v>
+      </c>
+      <c r="I7" s="222">
+        <v>50</v>
+      </c>
+      <c r="J7" s="223" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7" s="163"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="221">
+        <v>41</v>
+      </c>
+      <c r="N7" s="222">
+        <v>50</v>
+      </c>
+      <c r="O7" s="223" t="s">
+        <v>101</v>
+      </c>
+      <c r="P7" s="163"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="221">
+        <v>41</v>
+      </c>
+      <c r="S7" s="222">
+        <v>50</v>
+      </c>
+      <c r="T7" s="223" t="s">
+        <v>101</v>
+      </c>
+      <c r="U7" s="163"/>
+      <c r="V7" s="109"/>
+      <c r="W7" s="13">
+        <v>41</v>
+      </c>
+      <c r="X7" s="14">
+        <v>50</v>
+      </c>
+      <c r="Y7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z7" s="149"/>
+      <c r="AA7" s="187"/>
+      <c r="AB7" s="163"/>
+      <c r="AC7" s="109"/>
+      <c r="AD7" s="149"/>
+      <c r="AE7" s="187"/>
+      <c r="AF7" s="108"/>
+      <c r="AG7" s="109"/>
+      <c r="AH7" s="126"/>
+      <c r="AI7" s="112"/>
+      <c r="AJ7" s="129"/>
+      <c r="AK7" s="194"/>
+      <c r="AL7" s="81"/>
+      <c r="AM7" s="216"/>
+      <c r="AN7" s="109"/>
+      <c r="AO7" s="214"/>
+      <c r="AP7" s="92"/>
+      <c r="AQ7" s="214"/>
+      <c r="AR7" s="92"/>
+      <c r="AS7" s="214"/>
+      <c r="AT7" s="92"/>
+      <c r="AU7" s="13">
+        <v>41</v>
+      </c>
+      <c r="AV7" s="14">
+        <v>50</v>
+      </c>
+      <c r="AW7" s="234" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX7" s="97"/>
+      <c r="AY7" s="97"/>
+      <c r="AZ7" s="97"/>
+    </row>
+    <row r="8" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="209"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="221">
+        <v>51</v>
+      </c>
+      <c r="D8" s="222">
+        <v>60</v>
+      </c>
+      <c r="E8" s="223" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="163"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="221">
+        <v>51</v>
+      </c>
+      <c r="I8" s="222">
+        <v>60</v>
+      </c>
+      <c r="J8" s="223" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="163"/>
+      <c r="L8" s="109"/>
+      <c r="M8" s="221">
+        <v>51</v>
+      </c>
+      <c r="N8" s="222">
+        <v>60</v>
+      </c>
+      <c r="O8" s="223" t="s">
+        <v>111</v>
+      </c>
+      <c r="P8" s="163"/>
+      <c r="Q8" s="109"/>
+      <c r="R8" s="221">
+        <v>51</v>
+      </c>
+      <c r="S8" s="222">
+        <v>60</v>
+      </c>
+      <c r="T8" s="223" t="s">
+        <v>111</v>
+      </c>
+      <c r="U8" s="163"/>
+      <c r="V8" s="109"/>
+      <c r="W8" s="13">
+        <v>51</v>
+      </c>
+      <c r="X8" s="14">
+        <v>60</v>
+      </c>
+      <c r="Y8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z8" s="149"/>
+      <c r="AA8" s="187"/>
+      <c r="AB8" s="163"/>
+      <c r="AC8" s="109"/>
+      <c r="AD8" s="149"/>
+      <c r="AE8" s="187"/>
+      <c r="AF8" s="108"/>
+      <c r="AG8" s="109"/>
+      <c r="AH8" s="126"/>
+      <c r="AI8" s="112"/>
+      <c r="AJ8" s="129"/>
+      <c r="AK8" s="194"/>
+      <c r="AL8" s="81"/>
+      <c r="AM8" s="216"/>
+      <c r="AN8" s="109"/>
+      <c r="AO8" s="214"/>
+      <c r="AP8" s="92"/>
+      <c r="AQ8" s="214"/>
+      <c r="AR8" s="92"/>
+      <c r="AS8" s="214"/>
+      <c r="AT8" s="92"/>
+      <c r="AU8" s="13">
+        <v>51</v>
+      </c>
+      <c r="AV8" s="14">
+        <v>60</v>
+      </c>
+      <c r="AW8" s="234" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX8" s="97"/>
+      <c r="AY8" s="97"/>
+      <c r="AZ8" s="97"/>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A9" s="209"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="221">
+        <v>61</v>
+      </c>
+      <c r="D9" s="222">
+        <v>70</v>
+      </c>
+      <c r="E9" s="223" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="163"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="221">
+        <v>61</v>
+      </c>
+      <c r="I9" s="222">
+        <v>70</v>
+      </c>
+      <c r="J9" s="223" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="163"/>
+      <c r="L9" s="109"/>
+      <c r="M9" s="221">
+        <v>61</v>
+      </c>
+      <c r="N9" s="222">
+        <v>70</v>
+      </c>
+      <c r="O9" s="223" t="s">
+        <v>112</v>
+      </c>
+      <c r="P9" s="163"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="221">
+        <v>61</v>
+      </c>
+      <c r="S9" s="222">
+        <v>70</v>
+      </c>
+      <c r="T9" s="223" t="s">
+        <v>112</v>
+      </c>
+      <c r="U9" s="163"/>
+      <c r="V9" s="109"/>
+      <c r="W9" s="13">
+        <v>61</v>
+      </c>
+      <c r="X9" s="14">
+        <v>70</v>
+      </c>
+      <c r="Y9" s="238" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z9" s="149"/>
+      <c r="AA9" s="187"/>
+      <c r="AB9" s="163"/>
+      <c r="AC9" s="109"/>
+      <c r="AD9" s="149"/>
+      <c r="AE9" s="187"/>
+      <c r="AF9" s="108"/>
+      <c r="AG9" s="109"/>
+      <c r="AH9" s="126"/>
+      <c r="AI9" s="112"/>
+      <c r="AJ9" s="129"/>
+      <c r="AK9" s="194"/>
+      <c r="AL9" s="81"/>
+      <c r="AM9" s="216"/>
+      <c r="AN9" s="109"/>
+      <c r="AO9" s="214"/>
+      <c r="AP9" s="92"/>
+      <c r="AQ9" s="214"/>
+      <c r="AR9" s="92"/>
+      <c r="AS9" s="214"/>
+      <c r="AT9" s="92"/>
+      <c r="AU9" s="13">
+        <v>61</v>
+      </c>
+      <c r="AV9" s="14">
+        <v>70</v>
+      </c>
+      <c r="AW9" s="234" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX9" s="97"/>
+      <c r="AY9" s="97"/>
+      <c r="AZ9" s="97"/>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A10" s="209"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="221">
+        <v>71</v>
+      </c>
+      <c r="D10" s="222">
+        <v>80</v>
+      </c>
+      <c r="E10" s="223" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="163"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="221">
+        <v>71</v>
+      </c>
+      <c r="I10" s="222">
+        <v>80</v>
+      </c>
+      <c r="J10" s="223" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" s="163"/>
+      <c r="L10" s="109"/>
+      <c r="M10" s="221">
+        <v>71</v>
+      </c>
+      <c r="N10" s="222">
+        <v>80</v>
+      </c>
+      <c r="O10" s="223" t="s">
+        <v>113</v>
+      </c>
+      <c r="P10" s="163"/>
+      <c r="Q10" s="109"/>
+      <c r="R10" s="221">
+        <v>71</v>
+      </c>
+      <c r="S10" s="222">
+        <v>80</v>
+      </c>
+      <c r="T10" s="223" t="s">
+        <v>113</v>
+      </c>
+      <c r="U10" s="163"/>
+      <c r="V10" s="109"/>
+      <c r="W10" s="13">
+        <v>71</v>
+      </c>
+      <c r="X10" s="14">
+        <v>80</v>
+      </c>
+      <c r="Y10" s="239" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z10" s="149"/>
+      <c r="AA10" s="187"/>
+      <c r="AB10" s="163"/>
+      <c r="AC10" s="109"/>
+      <c r="AD10" s="149"/>
+      <c r="AE10" s="187"/>
+      <c r="AF10" s="108"/>
+      <c r="AG10" s="109"/>
+      <c r="AH10" s="126"/>
+      <c r="AI10" s="112"/>
+      <c r="AJ10" s="129"/>
+      <c r="AK10" s="194"/>
+      <c r="AL10" s="81"/>
+      <c r="AM10" s="216"/>
+      <c r="AN10" s="109"/>
+      <c r="AO10" s="214"/>
+      <c r="AP10" s="92"/>
+      <c r="AQ10" s="214"/>
+      <c r="AR10" s="92"/>
+      <c r="AS10" s="214"/>
+      <c r="AT10" s="92"/>
+      <c r="AU10" s="13">
+        <v>71</v>
+      </c>
+      <c r="AV10" s="14">
+        <v>80</v>
+      </c>
+      <c r="AW10" s="234"/>
+      <c r="AX10" s="97"/>
+      <c r="AY10" s="97"/>
+      <c r="AZ10" s="97"/>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A11" s="209"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="221">
+        <v>81</v>
+      </c>
+      <c r="D11" s="222">
+        <v>90</v>
+      </c>
+      <c r="E11" s="223" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="163"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="221">
+        <v>81</v>
+      </c>
+      <c r="I11" s="222">
+        <v>90</v>
+      </c>
+      <c r="J11" s="223" t="s">
+        <v>114</v>
+      </c>
+      <c r="K11" s="163"/>
+      <c r="L11" s="109"/>
+      <c r="M11" s="221">
+        <v>81</v>
+      </c>
+      <c r="N11" s="222">
+        <v>90</v>
+      </c>
+      <c r="O11" s="223" t="s">
+        <v>114</v>
+      </c>
+      <c r="P11" s="163"/>
+      <c r="Q11" s="109"/>
+      <c r="R11" s="221">
+        <v>81</v>
+      </c>
+      <c r="S11" s="222">
+        <v>90</v>
+      </c>
+      <c r="T11" s="223" t="s">
+        <v>114</v>
+      </c>
+      <c r="U11" s="163"/>
+      <c r="V11" s="109"/>
+      <c r="W11" s="13">
+        <v>81</v>
+      </c>
+      <c r="X11" s="14">
+        <v>90</v>
+      </c>
+      <c r="Y11" s="240">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="Z11" s="149"/>
+      <c r="AA11" s="187"/>
+      <c r="AB11" s="163"/>
+      <c r="AC11" s="109"/>
+      <c r="AD11" s="149"/>
+      <c r="AE11" s="187"/>
+      <c r="AF11" s="108"/>
+      <c r="AG11" s="109"/>
+      <c r="AH11" s="126"/>
+      <c r="AI11" s="112"/>
+      <c r="AJ11" s="129"/>
+      <c r="AK11" s="194"/>
+      <c r="AL11" s="81"/>
+      <c r="AM11" s="216"/>
+      <c r="AN11" s="109"/>
+      <c r="AO11" s="214"/>
+      <c r="AP11" s="92"/>
+      <c r="AQ11" s="214"/>
+      <c r="AR11" s="92"/>
+      <c r="AS11" s="214"/>
+      <c r="AT11" s="92"/>
+      <c r="AU11" s="13">
+        <v>81</v>
+      </c>
+      <c r="AV11" s="14">
+        <v>90</v>
+      </c>
+      <c r="AW11" s="234"/>
+      <c r="AX11" s="97"/>
+      <c r="AY11" s="97"/>
+      <c r="AZ11" s="97"/>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A12" s="209"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="221">
+        <v>91</v>
+      </c>
+      <c r="D12" s="222">
+        <v>100</v>
+      </c>
+      <c r="E12" s="223"/>
+      <c r="F12" s="163"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="221">
+        <v>91</v>
+      </c>
+      <c r="I12" s="222">
+        <v>100</v>
+      </c>
+      <c r="J12" s="223"/>
+      <c r="K12" s="163"/>
+      <c r="L12" s="109"/>
+      <c r="M12" s="221">
+        <v>91</v>
+      </c>
+      <c r="N12" s="222">
+        <v>100</v>
+      </c>
+      <c r="O12" s="223"/>
+      <c r="P12" s="163"/>
+      <c r="Q12" s="109"/>
+      <c r="R12" s="221">
+        <v>91</v>
+      </c>
+      <c r="S12" s="222">
+        <v>100</v>
+      </c>
+      <c r="T12" s="223"/>
+      <c r="U12" s="163"/>
+      <c r="V12" s="109"/>
+      <c r="W12" s="13">
+        <v>91</v>
+      </c>
+      <c r="X12" s="14">
+        <v>100</v>
+      </c>
+      <c r="Y12" s="239" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z12" s="149"/>
+      <c r="AA12" s="187"/>
+      <c r="AB12" s="163"/>
+      <c r="AC12" s="109"/>
+      <c r="AD12" s="149"/>
+      <c r="AE12" s="187"/>
+      <c r="AF12" s="108"/>
+      <c r="AG12" s="109"/>
+      <c r="AH12" s="126"/>
+      <c r="AI12" s="112"/>
+      <c r="AJ12" s="129"/>
+      <c r="AK12" s="194"/>
+      <c r="AL12" s="81"/>
+      <c r="AM12" s="216"/>
+      <c r="AN12" s="109"/>
+      <c r="AO12" s="214"/>
+      <c r="AP12" s="92"/>
+      <c r="AQ12" s="214"/>
+      <c r="AR12" s="92"/>
+      <c r="AS12" s="214"/>
+      <c r="AT12" s="92"/>
+      <c r="AU12" s="13">
+        <v>91</v>
+      </c>
+      <c r="AV12" s="14">
+        <v>100</v>
+      </c>
+      <c r="AW12" s="234"/>
+      <c r="AX12" s="97"/>
+      <c r="AY12" s="97"/>
+      <c r="AZ12" s="97"/>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A13" s="209"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="221">
+        <v>101</v>
+      </c>
+      <c r="D13" s="222">
+        <v>110</v>
+      </c>
+      <c r="E13" s="223"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="221">
+        <v>101</v>
+      </c>
+      <c r="I13" s="222">
+        <v>110</v>
+      </c>
+      <c r="J13" s="223"/>
+      <c r="K13" s="163"/>
+      <c r="L13" s="109"/>
+      <c r="M13" s="221">
+        <v>101</v>
+      </c>
+      <c r="N13" s="222">
+        <v>110</v>
+      </c>
+      <c r="O13" s="223"/>
+      <c r="P13" s="163"/>
+      <c r="Q13" s="109"/>
+      <c r="R13" s="221">
+        <v>101</v>
+      </c>
+      <c r="S13" s="222">
+        <v>110</v>
+      </c>
+      <c r="T13" s="223"/>
+      <c r="U13" s="163"/>
+      <c r="V13" s="109"/>
+      <c r="W13" s="13">
+        <v>101</v>
+      </c>
+      <c r="X13" s="14">
+        <v>110</v>
+      </c>
+      <c r="Y13" s="239" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z13" s="149"/>
+      <c r="AA13" s="187"/>
+      <c r="AB13" s="163"/>
+      <c r="AC13" s="109"/>
+      <c r="AD13" s="149"/>
+      <c r="AE13" s="187"/>
+      <c r="AF13" s="108"/>
+      <c r="AG13" s="109"/>
+      <c r="AH13" s="132"/>
+      <c r="AI13" s="134"/>
+      <c r="AJ13" s="130"/>
+      <c r="AK13" s="194"/>
+      <c r="AL13" s="81"/>
+      <c r="AM13" s="216"/>
+      <c r="AN13" s="109"/>
+      <c r="AO13" s="214"/>
+      <c r="AP13" s="92"/>
+      <c r="AQ13" s="214"/>
+      <c r="AR13" s="92"/>
+      <c r="AS13" s="214"/>
+      <c r="AT13" s="92"/>
+      <c r="AU13" s="13">
+        <v>101</v>
+      </c>
+      <c r="AV13" s="14">
+        <v>110</v>
+      </c>
+      <c r="AW13" s="234"/>
+      <c r="AX13" s="97"/>
+      <c r="AY13" s="97"/>
+      <c r="AZ13" s="97"/>
+    </row>
+    <row r="14" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="209"/>
+      <c r="B14" s="108"/>
+      <c r="C14" s="221">
+        <v>111</v>
+      </c>
+      <c r="D14" s="222">
+        <v>120</v>
+      </c>
+      <c r="E14" s="223"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="221">
+        <v>111</v>
+      </c>
+      <c r="I14" s="222">
+        <v>120</v>
+      </c>
+      <c r="J14" s="223"/>
+      <c r="K14" s="163"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="221">
+        <v>111</v>
+      </c>
+      <c r="N14" s="222">
+        <v>120</v>
+      </c>
+      <c r="O14" s="223"/>
+      <c r="P14" s="163"/>
+      <c r="Q14" s="109"/>
+      <c r="R14" s="221">
+        <v>111</v>
+      </c>
+      <c r="S14" s="222">
+        <v>120</v>
+      </c>
+      <c r="T14" s="223"/>
+      <c r="U14" s="163"/>
+      <c r="V14" s="109"/>
+      <c r="W14" s="13">
+        <v>111</v>
+      </c>
+      <c r="X14" s="14">
+        <v>120</v>
+      </c>
+      <c r="Y14" s="239" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z14" s="152"/>
+      <c r="AA14" s="188"/>
+      <c r="AB14" s="163"/>
+      <c r="AC14" s="109"/>
+      <c r="AD14" s="152"/>
+      <c r="AE14" s="188"/>
+      <c r="AF14" s="108"/>
+      <c r="AG14" s="109"/>
+      <c r="AH14" s="13">
+        <v>111</v>
+      </c>
+      <c r="AI14" s="14">
+        <v>120</v>
+      </c>
+      <c r="AJ14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK14" s="194"/>
+      <c r="AL14" s="81"/>
+      <c r="AM14" s="216"/>
+      <c r="AN14" s="109"/>
+      <c r="AO14" s="214"/>
+      <c r="AP14" s="92"/>
+      <c r="AQ14" s="214"/>
+      <c r="AR14" s="92"/>
+      <c r="AS14" s="214"/>
+      <c r="AT14" s="92"/>
+      <c r="AU14" s="13">
+        <v>111</v>
+      </c>
+      <c r="AV14" s="14">
+        <v>120</v>
+      </c>
+      <c r="AW14" s="234"/>
+      <c r="AX14" s="97"/>
+      <c r="AY14" s="97"/>
+      <c r="AZ14" s="97"/>
+    </row>
+    <row r="15" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="209"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="221">
+        <v>121</v>
+      </c>
+      <c r="D15" s="222">
+        <v>130</v>
+      </c>
+      <c r="E15" s="223"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="221">
+        <v>121</v>
+      </c>
+      <c r="I15" s="222">
+        <v>130</v>
+      </c>
+      <c r="J15" s="223"/>
+      <c r="K15" s="163"/>
+      <c r="L15" s="109"/>
+      <c r="M15" s="221">
+        <v>121</v>
+      </c>
+      <c r="N15" s="222">
+        <v>130</v>
+      </c>
+      <c r="O15" s="223"/>
+      <c r="P15" s="163"/>
+      <c r="Q15" s="109"/>
+      <c r="R15" s="221">
+        <v>121</v>
+      </c>
+      <c r="S15" s="222">
+        <v>130</v>
+      </c>
+      <c r="T15" s="223"/>
+      <c r="U15" s="163"/>
+      <c r="V15" s="109"/>
+      <c r="W15" s="13">
+        <v>120.833333333333</v>
+      </c>
+      <c r="X15" s="14">
+        <v>130</v>
+      </c>
+      <c r="Y15" s="241" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z15" s="75">
+        <v>127</v>
+      </c>
+      <c r="AA15" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB15" s="163"/>
+      <c r="AC15" s="109"/>
+      <c r="AD15" s="75">
+        <v>127</v>
+      </c>
+      <c r="AE15" s="73" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF15" s="108"/>
+      <c r="AG15" s="109"/>
+      <c r="AH15" s="131">
+        <v>120.833333333333</v>
+      </c>
+      <c r="AI15" s="133">
+        <v>200</v>
+      </c>
+      <c r="AJ15" s="80" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK15" s="194"/>
+      <c r="AL15" s="81"/>
+      <c r="AM15" s="216"/>
+      <c r="AN15" s="109"/>
+      <c r="AO15" s="214"/>
+      <c r="AP15" s="92"/>
+      <c r="AQ15" s="214"/>
+      <c r="AR15" s="92"/>
+      <c r="AS15" s="214"/>
+      <c r="AT15" s="92"/>
+      <c r="AU15" s="13">
+        <v>120.833333333333</v>
+      </c>
+      <c r="AV15" s="14">
+        <v>130</v>
+      </c>
+      <c r="AW15" s="234"/>
+      <c r="AX15" s="97"/>
+      <c r="AY15" s="97"/>
+      <c r="AZ15" s="97"/>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A16" s="209"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="221">
+        <v>131</v>
+      </c>
+      <c r="D16" s="222">
+        <v>140</v>
+      </c>
+      <c r="E16" s="223"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="221">
+        <v>131</v>
+      </c>
+      <c r="I16" s="222">
+        <v>140</v>
+      </c>
+      <c r="J16" s="223"/>
+      <c r="K16" s="163"/>
+      <c r="L16" s="109"/>
+      <c r="M16" s="221">
+        <v>131</v>
+      </c>
+      <c r="N16" s="222">
+        <v>140</v>
+      </c>
+      <c r="O16" s="223"/>
+      <c r="P16" s="163"/>
+      <c r="Q16" s="109"/>
+      <c r="R16" s="221">
+        <v>131</v>
+      </c>
+      <c r="S16" s="222">
+        <v>140</v>
+      </c>
+      <c r="T16" s="223"/>
+      <c r="U16" s="163"/>
+      <c r="V16" s="109"/>
+      <c r="W16" s="13">
+        <v>131</v>
+      </c>
+      <c r="X16" s="14">
+        <v>140</v>
+      </c>
+      <c r="Y16" s="242" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z16" s="148"/>
+      <c r="AA16" s="189" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB16" s="163"/>
+      <c r="AC16" s="109"/>
+      <c r="AD16" s="153">
+        <v>255</v>
+      </c>
+      <c r="AE16" s="189" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF16" s="108"/>
+      <c r="AG16" s="109"/>
+      <c r="AH16" s="126"/>
+      <c r="AI16" s="112"/>
+      <c r="AJ16" s="81"/>
+      <c r="AK16" s="194"/>
+      <c r="AL16" s="81"/>
+      <c r="AM16" s="216"/>
+      <c r="AN16" s="109"/>
+      <c r="AO16" s="214"/>
+      <c r="AP16" s="92"/>
+      <c r="AQ16" s="214"/>
+      <c r="AR16" s="92"/>
+      <c r="AS16" s="214"/>
+      <c r="AT16" s="92"/>
+      <c r="AU16" s="13">
+        <v>131</v>
+      </c>
+      <c r="AV16" s="14">
+        <v>140</v>
+      </c>
+      <c r="AW16" s="234"/>
+      <c r="AX16" s="97"/>
+      <c r="AY16" s="97"/>
+      <c r="AZ16" s="97"/>
+    </row>
+    <row r="17" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="209"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="221">
+        <v>141</v>
+      </c>
+      <c r="D17" s="222">
+        <v>150</v>
+      </c>
+      <c r="E17" s="223"/>
+      <c r="F17" s="164"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="221">
+        <v>141</v>
+      </c>
+      <c r="I17" s="222">
+        <v>150</v>
+      </c>
+      <c r="J17" s="223"/>
+      <c r="K17" s="164"/>
+      <c r="L17" s="165"/>
+      <c r="M17" s="221">
+        <v>141</v>
+      </c>
+      <c r="N17" s="222">
+        <v>150</v>
+      </c>
+      <c r="O17" s="223"/>
+      <c r="P17" s="164"/>
+      <c r="Q17" s="165"/>
+      <c r="R17" s="221">
+        <v>141</v>
+      </c>
+      <c r="S17" s="222">
+        <v>150</v>
+      </c>
+      <c r="T17" s="223"/>
+      <c r="U17" s="164"/>
+      <c r="V17" s="165"/>
+      <c r="W17" s="13">
+        <v>141</v>
+      </c>
+      <c r="X17" s="14">
+        <v>150</v>
+      </c>
+      <c r="Y17" s="243">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="Z17" s="149"/>
+      <c r="AA17" s="190"/>
+      <c r="AB17" s="185"/>
+      <c r="AC17" s="184"/>
+      <c r="AD17" s="154"/>
+      <c r="AE17" s="190"/>
+      <c r="AF17" s="183"/>
+      <c r="AG17" s="184"/>
+      <c r="AH17" s="126"/>
+      <c r="AI17" s="112"/>
+      <c r="AJ17" s="81"/>
+      <c r="AK17" s="194"/>
+      <c r="AL17" s="81"/>
+      <c r="AM17" s="217"/>
+      <c r="AN17" s="165"/>
+      <c r="AO17" s="214"/>
+      <c r="AP17" s="92"/>
+      <c r="AQ17" s="214"/>
+      <c r="AR17" s="92"/>
+      <c r="AS17" s="214"/>
+      <c r="AT17" s="92"/>
+      <c r="AU17" s="13">
+        <v>141</v>
+      </c>
+      <c r="AV17" s="14">
+        <v>150</v>
+      </c>
+      <c r="AW17" s="234"/>
+      <c r="AX17" s="97"/>
+      <c r="AY17" s="97"/>
+      <c r="AZ17" s="97"/>
+    </row>
+    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A18" s="209"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="221">
+        <v>151</v>
+      </c>
+      <c r="D18" s="222">
+        <v>160</v>
+      </c>
+      <c r="E18" s="224"/>
+      <c r="F18" s="201" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="140" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="221">
+        <v>151</v>
+      </c>
+      <c r="I18" s="222">
+        <v>160</v>
+      </c>
+      <c r="J18" s="224"/>
+      <c r="K18" s="159" t="s">
+        <v>90</v>
+      </c>
+      <c r="L18" s="140" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" s="221">
+        <v>151</v>
+      </c>
+      <c r="N18" s="222">
+        <v>160</v>
+      </c>
+      <c r="O18" s="224"/>
+      <c r="P18" s="159" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q18" s="140" t="s">
+        <v>67</v>
+      </c>
+      <c r="R18" s="221">
+        <v>151</v>
+      </c>
+      <c r="S18" s="222">
+        <v>160</v>
+      </c>
+      <c r="T18" s="224"/>
+      <c r="U18" s="159" t="s">
+        <v>92</v>
+      </c>
+      <c r="V18" s="140" t="s">
+        <v>80</v>
+      </c>
+      <c r="W18" s="13">
+        <v>150.833333333333</v>
+      </c>
+      <c r="X18" s="14">
+        <v>160</v>
+      </c>
+      <c r="Y18" s="242" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z18" s="149"/>
+      <c r="AA18" s="190"/>
+      <c r="AB18" s="204" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC18" s="136" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD18" s="154"/>
+      <c r="AE18" s="190"/>
+      <c r="AF18" s="198" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG18" s="136" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH18" s="126"/>
+      <c r="AI18" s="112"/>
+      <c r="AJ18" s="81"/>
+      <c r="AK18" s="194"/>
+      <c r="AL18" s="81"/>
+      <c r="AM18" s="178" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN18" s="140"/>
+      <c r="AO18" s="178" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP18" s="140"/>
+      <c r="AQ18" s="178" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR18" s="140"/>
+      <c r="AS18" s="178" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT18" s="140"/>
+      <c r="AU18" s="13">
+        <v>150.833333333333</v>
+      </c>
+      <c r="AV18" s="14">
+        <v>160</v>
+      </c>
+      <c r="AW18" s="234"/>
+      <c r="AX18" s="97"/>
+      <c r="AY18" s="97"/>
+      <c r="AZ18" s="97"/>
+    </row>
+    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A19" s="209"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="221">
+        <v>161</v>
+      </c>
+      <c r="D19" s="222">
+        <v>170</v>
+      </c>
+      <c r="E19" s="224"/>
+      <c r="F19" s="202"/>
+      <c r="G19" s="142"/>
+      <c r="H19" s="221">
+        <v>161</v>
+      </c>
+      <c r="I19" s="222">
+        <v>170</v>
+      </c>
+      <c r="J19" s="224"/>
+      <c r="K19" s="160"/>
+      <c r="L19" s="142"/>
+      <c r="M19" s="221">
+        <v>161</v>
+      </c>
+      <c r="N19" s="222">
+        <v>170</v>
+      </c>
+      <c r="O19" s="224"/>
+      <c r="P19" s="160"/>
+      <c r="Q19" s="142"/>
+      <c r="R19" s="221">
+        <v>161</v>
+      </c>
+      <c r="S19" s="222">
+        <v>170</v>
+      </c>
+      <c r="T19" s="224"/>
+      <c r="U19" s="160"/>
+      <c r="V19" s="142"/>
+      <c r="W19" s="13">
+        <v>161</v>
+      </c>
+      <c r="X19" s="14">
+        <v>170</v>
+      </c>
+      <c r="Y19" s="242" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z19" s="149"/>
+      <c r="AA19" s="190"/>
+      <c r="AB19" s="205"/>
+      <c r="AC19" s="137"/>
+      <c r="AD19" s="154"/>
+      <c r="AE19" s="190"/>
+      <c r="AF19" s="199"/>
+      <c r="AG19" s="137"/>
+      <c r="AH19" s="126"/>
+      <c r="AI19" s="112"/>
+      <c r="AJ19" s="81"/>
+      <c r="AK19" s="194"/>
+      <c r="AL19" s="81"/>
+      <c r="AM19" s="179"/>
+      <c r="AN19" s="142"/>
+      <c r="AO19" s="179"/>
+      <c r="AP19" s="142"/>
+      <c r="AQ19" s="179"/>
+      <c r="AR19" s="142"/>
+      <c r="AS19" s="179"/>
+      <c r="AT19" s="142"/>
+      <c r="AU19" s="13">
+        <v>161</v>
+      </c>
+      <c r="AV19" s="14">
+        <v>170</v>
+      </c>
+      <c r="AW19" s="234"/>
+      <c r="AX19" s="97"/>
+      <c r="AY19" s="97"/>
+      <c r="AZ19" s="97"/>
+    </row>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A20" s="209"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="221">
+        <v>171</v>
+      </c>
+      <c r="D20" s="222">
+        <v>180</v>
+      </c>
+      <c r="E20" s="224"/>
+      <c r="F20" s="202"/>
+      <c r="G20" s="142"/>
+      <c r="H20" s="221">
+        <v>171</v>
+      </c>
+      <c r="I20" s="222">
+        <v>180</v>
+      </c>
+      <c r="J20" s="224"/>
+      <c r="K20" s="160"/>
+      <c r="L20" s="142"/>
+      <c r="M20" s="221">
+        <v>171</v>
+      </c>
+      <c r="N20" s="222">
+        <v>180</v>
+      </c>
+      <c r="O20" s="224"/>
+      <c r="P20" s="160"/>
+      <c r="Q20" s="142"/>
+      <c r="R20" s="221">
+        <v>171</v>
+      </c>
+      <c r="S20" s="222">
+        <v>180</v>
+      </c>
+      <c r="T20" s="224"/>
+      <c r="U20" s="160"/>
+      <c r="V20" s="142"/>
+      <c r="W20" s="13">
+        <v>171</v>
+      </c>
+      <c r="X20" s="14">
+        <v>180</v>
+      </c>
+      <c r="Y20" s="242" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z20" s="149"/>
+      <c r="AA20" s="190"/>
+      <c r="AB20" s="205"/>
+      <c r="AC20" s="137"/>
+      <c r="AD20" s="154"/>
+      <c r="AE20" s="190"/>
+      <c r="AF20" s="199"/>
+      <c r="AG20" s="137"/>
+      <c r="AH20" s="126"/>
+      <c r="AI20" s="112"/>
+      <c r="AJ20" s="81"/>
+      <c r="AK20" s="194"/>
+      <c r="AL20" s="81"/>
+      <c r="AM20" s="179"/>
+      <c r="AN20" s="142"/>
+      <c r="AO20" s="179"/>
+      <c r="AP20" s="142"/>
+      <c r="AQ20" s="179"/>
+      <c r="AR20" s="142"/>
+      <c r="AS20" s="179"/>
+      <c r="AT20" s="142"/>
+      <c r="AU20" s="13">
+        <v>171</v>
+      </c>
+      <c r="AV20" s="14">
+        <v>180</v>
+      </c>
+      <c r="AW20" s="234"/>
+      <c r="AX20" s="97"/>
+      <c r="AY20" s="97"/>
+      <c r="AZ20" s="97"/>
+    </row>
+    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A21" s="209"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="221">
+        <v>181</v>
+      </c>
+      <c r="D21" s="222">
+        <v>190</v>
+      </c>
+      <c r="E21" s="224"/>
+      <c r="F21" s="202"/>
+      <c r="G21" s="142"/>
+      <c r="H21" s="221">
+        <v>181</v>
+      </c>
+      <c r="I21" s="222">
+        <v>190</v>
+      </c>
+      <c r="J21" s="224"/>
+      <c r="K21" s="160"/>
+      <c r="L21" s="142"/>
+      <c r="M21" s="221">
+        <v>181</v>
+      </c>
+      <c r="N21" s="222">
+        <v>190</v>
+      </c>
+      <c r="O21" s="224"/>
+      <c r="P21" s="160"/>
+      <c r="Q21" s="142"/>
+      <c r="R21" s="221">
+        <v>181</v>
+      </c>
+      <c r="S21" s="222">
+        <v>190</v>
+      </c>
+      <c r="T21" s="224"/>
+      <c r="U21" s="160"/>
+      <c r="V21" s="142"/>
+      <c r="W21" s="13">
+        <v>181</v>
+      </c>
+      <c r="X21" s="14">
+        <v>190</v>
+      </c>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="149"/>
+      <c r="AA21" s="190"/>
+      <c r="AB21" s="205"/>
+      <c r="AC21" s="137"/>
+      <c r="AD21" s="154"/>
+      <c r="AE21" s="190"/>
+      <c r="AF21" s="199"/>
+      <c r="AG21" s="137"/>
+      <c r="AH21" s="126"/>
+      <c r="AI21" s="112"/>
+      <c r="AJ21" s="81"/>
+      <c r="AK21" s="194"/>
+      <c r="AL21" s="81"/>
+      <c r="AM21" s="179"/>
+      <c r="AN21" s="142"/>
+      <c r="AO21" s="179"/>
+      <c r="AP21" s="142"/>
+      <c r="AQ21" s="179"/>
+      <c r="AR21" s="142"/>
+      <c r="AS21" s="179"/>
+      <c r="AT21" s="142"/>
+      <c r="AU21" s="13">
+        <v>181</v>
+      </c>
+      <c r="AV21" s="14">
+        <v>190</v>
+      </c>
+      <c r="AW21" s="234"/>
+      <c r="AX21" s="97"/>
+      <c r="AY21" s="97"/>
+      <c r="AZ21" s="97"/>
+    </row>
+    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A22" s="209"/>
+      <c r="B22" s="108"/>
+      <c r="C22" s="221">
+        <v>191</v>
+      </c>
+      <c r="D22" s="222">
+        <v>200</v>
+      </c>
+      <c r="E22" s="224"/>
+      <c r="F22" s="202"/>
+      <c r="G22" s="142"/>
+      <c r="H22" s="221">
+        <v>191</v>
+      </c>
+      <c r="I22" s="222">
+        <v>200</v>
+      </c>
+      <c r="J22" s="224"/>
+      <c r="K22" s="160"/>
+      <c r="L22" s="142"/>
+      <c r="M22" s="221">
+        <v>191</v>
+      </c>
+      <c r="N22" s="222">
+        <v>200</v>
+      </c>
+      <c r="O22" s="224"/>
+      <c r="P22" s="160"/>
+      <c r="Q22" s="142"/>
+      <c r="R22" s="221">
+        <v>191</v>
+      </c>
+      <c r="S22" s="222">
+        <v>200</v>
+      </c>
+      <c r="T22" s="224"/>
+      <c r="U22" s="160"/>
+      <c r="V22" s="142"/>
+      <c r="W22" s="13">
+        <v>191</v>
+      </c>
+      <c r="X22" s="14">
+        <v>200</v>
+      </c>
+      <c r="Y22" s="17"/>
+      <c r="Z22" s="149"/>
+      <c r="AA22" s="190"/>
+      <c r="AB22" s="205"/>
+      <c r="AC22" s="137"/>
+      <c r="AD22" s="154"/>
+      <c r="AE22" s="190"/>
+      <c r="AF22" s="199"/>
+      <c r="AG22" s="137"/>
+      <c r="AH22" s="132"/>
+      <c r="AI22" s="134"/>
+      <c r="AJ22" s="135"/>
+      <c r="AK22" s="194"/>
+      <c r="AL22" s="81"/>
+      <c r="AM22" s="179"/>
+      <c r="AN22" s="142"/>
+      <c r="AO22" s="179"/>
+      <c r="AP22" s="142"/>
+      <c r="AQ22" s="179"/>
+      <c r="AR22" s="142"/>
+      <c r="AS22" s="179"/>
+      <c r="AT22" s="142"/>
+      <c r="AU22" s="13">
+        <v>191</v>
+      </c>
+      <c r="AV22" s="14">
+        <v>200</v>
+      </c>
+      <c r="AW22" s="234"/>
+      <c r="AX22" s="97"/>
+      <c r="AY22" s="97"/>
+      <c r="AZ22" s="97"/>
+    </row>
+    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A23" s="209"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="221">
+        <v>201</v>
+      </c>
+      <c r="D23" s="222">
+        <v>210</v>
+      </c>
+      <c r="E23" s="224"/>
+      <c r="F23" s="202"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="221">
+        <v>201</v>
+      </c>
+      <c r="I23" s="222">
+        <v>210</v>
+      </c>
+      <c r="J23" s="224"/>
+      <c r="K23" s="160"/>
+      <c r="L23" s="142"/>
+      <c r="M23" s="221">
+        <v>201</v>
+      </c>
+      <c r="N23" s="222">
+        <v>210</v>
+      </c>
+      <c r="O23" s="224"/>
+      <c r="P23" s="160"/>
+      <c r="Q23" s="142"/>
+      <c r="R23" s="221">
+        <v>201</v>
+      </c>
+      <c r="S23" s="222">
+        <v>210</v>
+      </c>
+      <c r="T23" s="224"/>
+      <c r="U23" s="160"/>
+      <c r="V23" s="142"/>
+      <c r="W23" s="13">
+        <v>201</v>
+      </c>
+      <c r="X23" s="14">
+        <v>210</v>
+      </c>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="149"/>
+      <c r="AA23" s="190"/>
+      <c r="AB23" s="205"/>
+      <c r="AC23" s="137"/>
+      <c r="AD23" s="154"/>
+      <c r="AE23" s="190"/>
+      <c r="AF23" s="199"/>
+      <c r="AG23" s="137"/>
+      <c r="AH23" s="131">
+        <v>201</v>
+      </c>
+      <c r="AI23" s="133">
+        <v>255</v>
+      </c>
+      <c r="AJ23" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK23" s="194"/>
+      <c r="AL23" s="81"/>
+      <c r="AM23" s="179"/>
+      <c r="AN23" s="142"/>
+      <c r="AO23" s="179"/>
+      <c r="AP23" s="142"/>
+      <c r="AQ23" s="179"/>
+      <c r="AR23" s="142"/>
+      <c r="AS23" s="179"/>
+      <c r="AT23" s="142"/>
+      <c r="AU23" s="13">
+        <v>201</v>
+      </c>
+      <c r="AV23" s="14">
+        <v>210</v>
+      </c>
+      <c r="AW23" s="234"/>
+      <c r="AX23" s="97"/>
+      <c r="AY23" s="97"/>
+      <c r="AZ23" s="97"/>
+    </row>
+    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A24" s="209"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="221">
+        <v>211</v>
+      </c>
+      <c r="D24" s="222">
+        <v>220</v>
+      </c>
+      <c r="E24" s="224"/>
+      <c r="F24" s="202"/>
+      <c r="G24" s="142"/>
+      <c r="H24" s="221">
+        <v>211</v>
+      </c>
+      <c r="I24" s="222">
+        <v>220</v>
+      </c>
+      <c r="J24" s="224"/>
+      <c r="K24" s="160"/>
+      <c r="L24" s="142"/>
+      <c r="M24" s="221">
+        <v>211</v>
+      </c>
+      <c r="N24" s="222">
+        <v>220</v>
+      </c>
+      <c r="O24" s="224"/>
+      <c r="P24" s="160"/>
+      <c r="Q24" s="142"/>
+      <c r="R24" s="221">
+        <v>211</v>
+      </c>
+      <c r="S24" s="222">
+        <v>220</v>
+      </c>
+      <c r="T24" s="224"/>
+      <c r="U24" s="160"/>
+      <c r="V24" s="142"/>
+      <c r="W24" s="13">
+        <v>210</v>
+      </c>
+      <c r="X24" s="14">
+        <v>220</v>
+      </c>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="149"/>
+      <c r="AA24" s="190"/>
+      <c r="AB24" s="205"/>
+      <c r="AC24" s="137"/>
+      <c r="AD24" s="154"/>
+      <c r="AE24" s="190"/>
+      <c r="AF24" s="199"/>
+      <c r="AG24" s="137"/>
+      <c r="AH24" s="126"/>
+      <c r="AI24" s="112"/>
+      <c r="AJ24" s="81"/>
+      <c r="AK24" s="194"/>
+      <c r="AL24" s="81"/>
+      <c r="AM24" s="179"/>
+      <c r="AN24" s="142"/>
+      <c r="AO24" s="179"/>
+      <c r="AP24" s="142"/>
+      <c r="AQ24" s="179"/>
+      <c r="AR24" s="142"/>
+      <c r="AS24" s="179"/>
+      <c r="AT24" s="142"/>
+      <c r="AU24" s="13">
+        <v>210</v>
+      </c>
+      <c r="AV24" s="14">
+        <v>220</v>
+      </c>
+      <c r="AW24" s="234"/>
+      <c r="AX24" s="97"/>
+      <c r="AY24" s="97"/>
+      <c r="AZ24" s="97"/>
+    </row>
+    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A25" s="209"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="221">
+        <v>221</v>
+      </c>
+      <c r="D25" s="222">
+        <v>230</v>
+      </c>
+      <c r="E25" s="224"/>
+      <c r="F25" s="202"/>
+      <c r="G25" s="142"/>
+      <c r="H25" s="221">
+        <v>221</v>
+      </c>
+      <c r="I25" s="222">
+        <v>230</v>
+      </c>
+      <c r="J25" s="224"/>
+      <c r="K25" s="160"/>
+      <c r="L25" s="142"/>
+      <c r="M25" s="221">
+        <v>221</v>
+      </c>
+      <c r="N25" s="222">
+        <v>230</v>
+      </c>
+      <c r="O25" s="224"/>
+      <c r="P25" s="160"/>
+      <c r="Q25" s="142"/>
+      <c r="R25" s="221">
+        <v>221</v>
+      </c>
+      <c r="S25" s="222">
+        <v>230</v>
+      </c>
+      <c r="T25" s="224"/>
+      <c r="U25" s="160"/>
+      <c r="V25" s="142"/>
+      <c r="W25" s="13">
+        <v>221</v>
+      </c>
+      <c r="X25" s="14">
+        <v>230</v>
+      </c>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="149"/>
+      <c r="AA25" s="190"/>
+      <c r="AB25" s="205"/>
+      <c r="AC25" s="137"/>
+      <c r="AD25" s="154"/>
+      <c r="AE25" s="190"/>
+      <c r="AF25" s="199"/>
+      <c r="AG25" s="137"/>
+      <c r="AH25" s="126"/>
+      <c r="AI25" s="112"/>
+      <c r="AJ25" s="81"/>
+      <c r="AK25" s="194"/>
+      <c r="AL25" s="81"/>
+      <c r="AM25" s="179"/>
+      <c r="AN25" s="142"/>
+      <c r="AO25" s="179"/>
+      <c r="AP25" s="142"/>
+      <c r="AQ25" s="179"/>
+      <c r="AR25" s="142"/>
+      <c r="AS25" s="179"/>
+      <c r="AT25" s="142"/>
+      <c r="AU25" s="13">
+        <v>221</v>
+      </c>
+      <c r="AV25" s="14">
+        <v>230</v>
+      </c>
+      <c r="AW25" s="234"/>
+      <c r="AX25" s="97"/>
+      <c r="AY25" s="97"/>
+      <c r="AZ25" s="97"/>
+    </row>
+    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A26" s="209"/>
+      <c r="B26" s="108"/>
+      <c r="C26" s="221">
+        <v>231</v>
+      </c>
+      <c r="D26" s="222">
+        <v>240</v>
+      </c>
+      <c r="E26" s="224"/>
+      <c r="F26" s="202"/>
+      <c r="G26" s="142"/>
+      <c r="H26" s="221">
+        <v>231</v>
+      </c>
+      <c r="I26" s="222">
+        <v>240</v>
+      </c>
+      <c r="J26" s="224"/>
+      <c r="K26" s="160"/>
+      <c r="L26" s="142"/>
+      <c r="M26" s="221">
+        <v>231</v>
+      </c>
+      <c r="N26" s="222">
+        <v>240</v>
+      </c>
+      <c r="O26" s="224"/>
+      <c r="P26" s="160"/>
+      <c r="Q26" s="142"/>
+      <c r="R26" s="221">
+        <v>231</v>
+      </c>
+      <c r="S26" s="222">
+        <v>240</v>
+      </c>
+      <c r="T26" s="224"/>
+      <c r="U26" s="160"/>
+      <c r="V26" s="142"/>
+      <c r="W26" s="13">
+        <v>231</v>
+      </c>
+      <c r="X26" s="14">
+        <v>240</v>
+      </c>
+      <c r="Y26" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z26" s="149"/>
+      <c r="AA26" s="190"/>
+      <c r="AB26" s="205"/>
+      <c r="AC26" s="137"/>
+      <c r="AD26" s="154"/>
+      <c r="AE26" s="190"/>
+      <c r="AF26" s="199"/>
+      <c r="AG26" s="137"/>
+      <c r="AH26" s="126"/>
+      <c r="AI26" s="112"/>
+      <c r="AJ26" s="81"/>
+      <c r="AK26" s="194"/>
+      <c r="AL26" s="81"/>
+      <c r="AM26" s="179"/>
+      <c r="AN26" s="142"/>
+      <c r="AO26" s="179"/>
+      <c r="AP26" s="142"/>
+      <c r="AQ26" s="179"/>
+      <c r="AR26" s="142"/>
+      <c r="AS26" s="179"/>
+      <c r="AT26" s="142"/>
+      <c r="AU26" s="13">
+        <v>231</v>
+      </c>
+      <c r="AV26" s="14">
+        <v>240</v>
+      </c>
+      <c r="AW26" s="234"/>
+      <c r="AX26" s="97"/>
+      <c r="AY26" s="97"/>
+      <c r="AZ26" s="97"/>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A27" s="209"/>
+      <c r="B27" s="108"/>
+      <c r="C27" s="221">
+        <v>241</v>
+      </c>
+      <c r="D27" s="222">
+        <v>250</v>
+      </c>
+      <c r="E27" s="224"/>
+      <c r="F27" s="202"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="221">
+        <v>241</v>
+      </c>
+      <c r="I27" s="222">
+        <v>250</v>
+      </c>
+      <c r="J27" s="224"/>
+      <c r="K27" s="160"/>
+      <c r="L27" s="142"/>
+      <c r="M27" s="221">
+        <v>241</v>
+      </c>
+      <c r="N27" s="222">
+        <v>250</v>
+      </c>
+      <c r="O27" s="224"/>
+      <c r="P27" s="160"/>
+      <c r="Q27" s="142"/>
+      <c r="R27" s="221">
+        <v>241</v>
+      </c>
+      <c r="S27" s="222">
+        <v>250</v>
+      </c>
+      <c r="T27" s="224"/>
+      <c r="U27" s="160"/>
+      <c r="V27" s="142"/>
+      <c r="W27" s="13">
+        <v>241</v>
+      </c>
+      <c r="X27" s="14">
+        <v>250</v>
+      </c>
+      <c r="Y27" s="71" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z27" s="150"/>
+      <c r="AA27" s="190"/>
+      <c r="AB27" s="205"/>
+      <c r="AC27" s="137"/>
+      <c r="AD27" s="154"/>
+      <c r="AE27" s="190"/>
+      <c r="AF27" s="199"/>
+      <c r="AG27" s="137"/>
+      <c r="AH27" s="126"/>
+      <c r="AI27" s="112"/>
+      <c r="AJ27" s="81"/>
+      <c r="AK27" s="194"/>
+      <c r="AL27" s="81"/>
+      <c r="AM27" s="179"/>
+      <c r="AN27" s="142"/>
+      <c r="AO27" s="179"/>
+      <c r="AP27" s="142"/>
+      <c r="AQ27" s="179"/>
+      <c r="AR27" s="142"/>
+      <c r="AS27" s="179"/>
+      <c r="AT27" s="142"/>
+      <c r="AU27" s="13">
+        <v>241</v>
+      </c>
+      <c r="AV27" s="14">
+        <v>250</v>
+      </c>
+      <c r="AW27" s="234"/>
+      <c r="AX27" s="97"/>
+      <c r="AY27" s="97"/>
+      <c r="AZ27" s="97"/>
+    </row>
+    <row r="28" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="210"/>
+      <c r="B28" s="211"/>
+      <c r="C28" s="225">
+        <v>251</v>
+      </c>
+      <c r="D28" s="226">
+        <v>255</v>
+      </c>
+      <c r="E28" s="227"/>
+      <c r="F28" s="203"/>
+      <c r="G28" s="144"/>
+      <c r="H28" s="225">
+        <v>251</v>
+      </c>
+      <c r="I28" s="226">
+        <v>255</v>
+      </c>
+      <c r="J28" s="227"/>
+      <c r="K28" s="161"/>
+      <c r="L28" s="144"/>
+      <c r="M28" s="225">
+        <v>251</v>
+      </c>
+      <c r="N28" s="226">
+        <v>255</v>
+      </c>
+      <c r="O28" s="227"/>
+      <c r="P28" s="161"/>
+      <c r="Q28" s="144"/>
+      <c r="R28" s="225">
+        <v>251</v>
+      </c>
+      <c r="S28" s="226">
+        <v>255</v>
+      </c>
+      <c r="T28" s="227"/>
+      <c r="U28" s="161"/>
+      <c r="V28" s="144"/>
+      <c r="W28" s="59">
+        <v>251</v>
+      </c>
+      <c r="X28" s="53">
+        <v>255</v>
+      </c>
+      <c r="Y28" s="72"/>
+      <c r="Z28" s="76">
+        <v>255</v>
+      </c>
+      <c r="AA28" s="191"/>
+      <c r="AB28" s="206"/>
+      <c r="AC28" s="138"/>
+      <c r="AD28" s="155"/>
+      <c r="AE28" s="191"/>
+      <c r="AF28" s="200"/>
+      <c r="AG28" s="137"/>
+      <c r="AH28" s="126"/>
+      <c r="AI28" s="112"/>
+      <c r="AJ28" s="81"/>
+      <c r="AK28" s="196"/>
+      <c r="AL28" s="82"/>
+      <c r="AM28" s="180"/>
+      <c r="AN28" s="144"/>
+      <c r="AO28" s="180"/>
+      <c r="AP28" s="144"/>
+      <c r="AQ28" s="180"/>
+      <c r="AR28" s="144"/>
+      <c r="AS28" s="180"/>
+      <c r="AT28" s="144"/>
+      <c r="AU28" s="235">
+        <v>251</v>
+      </c>
+      <c r="AV28" s="236">
+        <v>255</v>
+      </c>
+      <c r="AW28" s="237" t="s">
+        <v>118</v>
+      </c>
+      <c r="AX28" s="98"/>
+      <c r="AY28" s="98"/>
+      <c r="AZ28" s="98"/>
+    </row>
+    <row r="29" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="58">
+        <v>-1</v>
+      </c>
+      <c r="C29" s="169">
+        <v>0</v>
+      </c>
+      <c r="D29" s="170"/>
+      <c r="E29" s="170"/>
+      <c r="F29" s="171"/>
+      <c r="G29" s="168"/>
+      <c r="H29" s="166">
+        <v>1</v>
+      </c>
+      <c r="I29" s="171"/>
+      <c r="J29" s="171"/>
+      <c r="K29" s="171"/>
+      <c r="L29" s="168"/>
+      <c r="M29" s="166">
+        <v>2</v>
+      </c>
+      <c r="N29" s="171"/>
+      <c r="O29" s="171"/>
+      <c r="P29" s="171"/>
+      <c r="Q29" s="168"/>
+      <c r="R29" s="166">
+        <v>3</v>
+      </c>
+      <c r="S29" s="171"/>
+      <c r="T29" s="171"/>
+      <c r="U29" s="171"/>
+      <c r="V29" s="168"/>
+      <c r="W29" s="166">
+        <v>4</v>
+      </c>
+      <c r="X29" s="167"/>
+      <c r="Y29" s="168"/>
+      <c r="Z29" s="174">
+        <v>5</v>
+      </c>
+      <c r="AA29" s="170"/>
+      <c r="AB29" s="171"/>
+      <c r="AC29" s="173"/>
+      <c r="AD29" s="172">
+        <v>6</v>
+      </c>
+      <c r="AE29" s="171"/>
+      <c r="AF29" s="171"/>
+      <c r="AG29" s="173"/>
+      <c r="AH29" s="166">
+        <v>7</v>
+      </c>
+      <c r="AI29" s="167"/>
+      <c r="AJ29" s="168"/>
+      <c r="AK29" s="166">
+        <v>8</v>
+      </c>
+      <c r="AL29" s="168"/>
+      <c r="AM29" s="174">
+        <v>9</v>
+      </c>
+      <c r="AN29" s="207"/>
+      <c r="AO29" s="172">
+        <v>10</v>
+      </c>
+      <c r="AP29" s="173"/>
+      <c r="AQ29" s="172">
+        <v>11</v>
+      </c>
+      <c r="AR29" s="173"/>
+      <c r="AS29" s="172">
+        <v>12</v>
+      </c>
+      <c r="AT29" s="173"/>
+      <c r="AU29" s="228">
+        <v>13</v>
+      </c>
+      <c r="AV29" s="229"/>
+      <c r="AW29" s="230"/>
+      <c r="AX29" s="231">
+        <v>14</v>
+      </c>
+      <c r="AY29" s="231">
+        <v>15</v>
+      </c>
+      <c r="AZ29" s="231">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="Y30" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="Y31" s="50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="Y32" s="57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="23:39" x14ac:dyDescent="0.25">
+      <c r="W33" s="212" t="s">
+        <v>95</v>
+      </c>
+      <c r="X33" s="212"/>
+      <c r="Y33" s="212"/>
+      <c r="Z33" s="212"/>
+      <c r="AA33" s="212"/>
+      <c r="AB33" s="212"/>
+      <c r="AC33" s="212"/>
+      <c r="AD33" s="212"/>
+      <c r="AE33" s="212"/>
+      <c r="AF33" s="212"/>
+      <c r="AG33" s="212"/>
+      <c r="AH33" s="212"/>
+      <c r="AI33" s="212"/>
+      <c r="AJ33" s="212"/>
+      <c r="AK33" s="212"/>
+      <c r="AL33" s="212"/>
+      <c r="AM33" s="212"/>
+    </row>
+    <row r="34" spans="23:39" x14ac:dyDescent="0.25">
+      <c r="W34" s="212"/>
+      <c r="X34" s="212"/>
+      <c r="Y34" s="212"/>
+      <c r="Z34" s="212"/>
+      <c r="AA34" s="212"/>
+      <c r="AB34" s="212"/>
+      <c r="AC34" s="212"/>
+      <c r="AD34" s="212"/>
+      <c r="AE34" s="212"/>
+      <c r="AF34" s="212"/>
+      <c r="AG34" s="212"/>
+      <c r="AH34" s="212"/>
+      <c r="AI34" s="212"/>
+      <c r="AJ34" s="212"/>
+      <c r="AK34" s="212"/>
+      <c r="AL34" s="212"/>
+      <c r="AM34" s="212"/>
+    </row>
+    <row r="35" spans="23:39" x14ac:dyDescent="0.25">
+      <c r="W35" s="212"/>
+      <c r="X35" s="212"/>
+      <c r="Y35" s="212"/>
+      <c r="Z35" s="212"/>
+      <c r="AA35" s="212"/>
+      <c r="AB35" s="212"/>
+      <c r="AC35" s="212"/>
+      <c r="AD35" s="212"/>
+      <c r="AE35" s="212"/>
+      <c r="AF35" s="212"/>
+      <c r="AG35" s="212"/>
+      <c r="AH35" s="212"/>
+      <c r="AI35" s="212"/>
+      <c r="AJ35" s="212"/>
+      <c r="AK35" s="212"/>
+      <c r="AL35" s="212"/>
+      <c r="AM35" s="212"/>
+    </row>
+    <row r="36" spans="23:39" x14ac:dyDescent="0.25">
+      <c r="W36" s="212"/>
+      <c r="X36" s="212"/>
+      <c r="Y36" s="212"/>
+      <c r="Z36" s="212"/>
+      <c r="AA36" s="212"/>
+      <c r="AB36" s="212"/>
+      <c r="AC36" s="212"/>
+      <c r="AD36" s="212"/>
+      <c r="AE36" s="212"/>
+      <c r="AF36" s="212"/>
+      <c r="AG36" s="212"/>
+      <c r="AH36" s="212"/>
+      <c r="AI36" s="212"/>
+      <c r="AJ36" s="212"/>
+      <c r="AK36" s="212"/>
+      <c r="AL36" s="212"/>
+      <c r="AM36" s="212"/>
+    </row>
+    <row r="37" spans="23:39" x14ac:dyDescent="0.25">
+      <c r="W37" s="212"/>
+      <c r="X37" s="212"/>
+      <c r="Y37" s="212"/>
+      <c r="Z37" s="212"/>
+      <c r="AA37" s="212"/>
+      <c r="AB37" s="212"/>
+      <c r="AC37" s="212"/>
+      <c r="AD37" s="212"/>
+      <c r="AE37" s="212"/>
+      <c r="AF37" s="212"/>
+      <c r="AG37" s="212"/>
+      <c r="AH37" s="212"/>
+      <c r="AI37" s="212"/>
+      <c r="AJ37" s="212"/>
+      <c r="AK37" s="212"/>
+      <c r="AL37" s="212"/>
+      <c r="AM37" s="212"/>
+    </row>
+  </sheetData>
+  <mergeCells count="102">
+    <mergeCell ref="AS29:AT29"/>
+    <mergeCell ref="AU29:AW29"/>
+    <mergeCell ref="W33:AM37"/>
+    <mergeCell ref="AD29:AG29"/>
+    <mergeCell ref="AH29:AJ29"/>
+    <mergeCell ref="AK29:AL29"/>
+    <mergeCell ref="AM29:AN29"/>
+    <mergeCell ref="AO29:AP29"/>
+    <mergeCell ref="AQ29:AR29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="M29:Q29"/>
+    <mergeCell ref="R29:V29"/>
+    <mergeCell ref="W29:Y29"/>
+    <mergeCell ref="Z29:AC29"/>
+    <mergeCell ref="U18:U28"/>
+    <mergeCell ref="V18:V28"/>
+    <mergeCell ref="AB18:AB28"/>
+    <mergeCell ref="AC18:AC28"/>
+    <mergeCell ref="AF18:AF28"/>
+    <mergeCell ref="AG18:AG28"/>
+    <mergeCell ref="Z16:Z27"/>
+    <mergeCell ref="AA16:AA28"/>
+    <mergeCell ref="AD16:AD28"/>
+    <mergeCell ref="AE16:AE28"/>
+    <mergeCell ref="F18:F28"/>
+    <mergeCell ref="G18:G28"/>
+    <mergeCell ref="K18:K28"/>
+    <mergeCell ref="L18:L28"/>
+    <mergeCell ref="P18:P28"/>
+    <mergeCell ref="Q18:Q28"/>
+    <mergeCell ref="AY3:AY28"/>
+    <mergeCell ref="AZ3:AZ28"/>
+    <mergeCell ref="Z4:Z14"/>
+    <mergeCell ref="AD4:AD14"/>
+    <mergeCell ref="AH6:AH13"/>
+    <mergeCell ref="AI6:AI13"/>
+    <mergeCell ref="AJ6:AJ13"/>
+    <mergeCell ref="AH15:AH22"/>
+    <mergeCell ref="AI15:AI22"/>
+    <mergeCell ref="AJ15:AJ22"/>
+    <mergeCell ref="AP3:AP17"/>
+    <mergeCell ref="AQ3:AQ17"/>
+    <mergeCell ref="AR3:AR17"/>
+    <mergeCell ref="AS3:AS17"/>
+    <mergeCell ref="AT3:AT17"/>
+    <mergeCell ref="AX3:AX28"/>
+    <mergeCell ref="AO18:AP28"/>
+    <mergeCell ref="AQ18:AR28"/>
+    <mergeCell ref="AS18:AT28"/>
+    <mergeCell ref="AF3:AG17"/>
+    <mergeCell ref="AK3:AK28"/>
+    <mergeCell ref="AL3:AL28"/>
+    <mergeCell ref="AM3:AM17"/>
+    <mergeCell ref="AN3:AN17"/>
+    <mergeCell ref="AO3:AO17"/>
+    <mergeCell ref="AM18:AN28"/>
+    <mergeCell ref="AH23:AH28"/>
+    <mergeCell ref="AI23:AI28"/>
+    <mergeCell ref="AJ23:AJ28"/>
+    <mergeCell ref="AU2:AW2"/>
+    <mergeCell ref="A3:A28"/>
+    <mergeCell ref="B3:B28"/>
+    <mergeCell ref="F3:G17"/>
+    <mergeCell ref="K3:L17"/>
+    <mergeCell ref="P3:Q17"/>
+    <mergeCell ref="U3:V17"/>
+    <mergeCell ref="AA3:AA14"/>
+    <mergeCell ref="AB3:AC17"/>
+    <mergeCell ref="AE3:AE14"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="AU1:AW1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>

</xml_diff>